<commit_message>
updated true odds calclulator
</commit_message>
<xml_diff>
--- a/CS generator.xlsx
+++ b/CS generator.xlsx
@@ -346,22 +346,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E55"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3">
-        <v>0.68586426914152976</v>
+        <v>2.3649805869074494</v>
       </c>
       <c r="B1" s="3">
-        <v>0.94694895591647588</v>
+        <v>1.2953769751693047</v>
       </c>
       <c r="C1" s="1">
         <f>ROUND(A1,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1">
         <f>ROUND(B1,0)</f>
@@ -369,59 +369,59 @@
       </c>
       <c r="E1" s="2" t="str">
         <f>CONCATENATE(C1,"-",D1)</f>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>0.93966545454545791</v>
+        <v>1.573226666666663</v>
       </c>
       <c r="B2" s="3">
-        <v>0.18666666666666656</v>
+        <v>0.91941818181817969</v>
       </c>
       <c r="C2" s="1">
         <f t="shared" ref="C2:C5" si="0">ROUND(A2,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1">
         <f t="shared" ref="D2:D5" si="1">ROUND(B2,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="str">
         <f t="shared" ref="E2:E5" si="2">CONCATENATE(C2,"-",D2)</f>
-        <v>1-0</v>
+        <v>2-1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>0.81550545454545764</v>
+        <v>2.1194699999999953</v>
       </c>
       <c r="B3" s="3">
-        <v>0.93469090909090857</v>
+        <v>0.49840909090908969</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>1-1</v>
+        <v>2-0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>1.4456380510440803</v>
+        <v>1.5260000000000045</v>
       </c>
       <c r="B4" s="3">
-        <v>1.331175870069609</v>
+        <v>0.84236574074074266</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="1"/>
@@ -429,15 +429,15 @@
       </c>
       <c r="E4" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>1.6177378190255183</v>
+        <v>2.0208833333333387</v>
       </c>
       <c r="B5" s="3">
-        <v>0.65558004640371403</v>
+        <v>1.2306149999999998</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
@@ -454,10 +454,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>0.51069605568445353</v>
+        <v>1.0979200000000029</v>
       </c>
       <c r="B6" s="3">
-        <v>1.9063127610208868</v>
+        <v>0.17445499999999997</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" ref="C6:C10" si="3">ROUND(A6,0)</f>
@@ -465,23 +465,23 @@
       </c>
       <c r="D6" s="1">
         <f t="shared" ref="D6:D10" si="4">ROUND(B6,0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" ref="E6:E11" si="5">CONCATENATE(C6,"-",D6)</f>
-        <v>1-2</v>
+        <v>1-0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>1.009785382830624</v>
+        <v>2.7336066666666738</v>
       </c>
       <c r="B7" s="3">
-        <v>0.53358515081206648</v>
+        <v>1.0938799999999997</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="4"/>
@@ -489,39 +489,39 @@
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>1-1</v>
+        <v>3-1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>1.8886948955916427</v>
+        <v>0.95776000000000239</v>
       </c>
       <c r="B8" s="3">
-        <v>1.2538997679814419</v>
+        <v>0.33947999999999995</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>2-1</v>
+        <v>1-0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>2.6091125290023141</v>
+        <v>1.6960333333333377</v>
       </c>
       <c r="B9" s="3">
-        <v>0.90577726218097698</v>
+        <v>0.85283999999999993</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="4"/>
@@ -529,19 +529,19 @@
       </c>
       <c r="E9" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>3-1</v>
+        <v>2-1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>1.0982366589327122</v>
+        <v>0.12084210526315786</v>
       </c>
       <c r="B10" s="3">
-        <v>1.6073429234338792</v>
+        <v>1.7362526315789488</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="4"/>
@@ -549,99 +549,99 @@
       </c>
       <c r="E10" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>0-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>1.0328654292343364</v>
+        <v>0.41891929824561402</v>
       </c>
       <c r="B11" s="3">
-        <v>1.8377777262181023</v>
+        <v>3.9065684210526346</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" ref="C11" si="6">ROUND(A11,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" ref="D11" si="7">ROUND(B11,0)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E11" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>1-2</v>
+        <v>0-4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>1.6147087962962927</v>
+        <v>0.7492210526315789</v>
       </c>
       <c r="B12" s="3">
-        <v>1.2344444444444433</v>
+        <v>2.9619473684210553</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" ref="C12:C75" si="8">ROUND(A12,0)</f>
-        <v>2</v>
+        <f t="shared" ref="C12:C15" si="8">ROUND(A12,0)</f>
+        <v>1</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" ref="D12:D75" si="9">ROUND(B12,0)</f>
-        <v>1</v>
+        <f t="shared" ref="D12:D15" si="9">ROUND(B12,0)</f>
+        <v>3</v>
       </c>
       <c r="E12" s="2" t="str">
-        <f t="shared" ref="E12:E75" si="10">CONCATENATE(C12,"-",D12)</f>
-        <v>2-1</v>
+        <f t="shared" ref="E12:E15" si="10">CONCATENATE(C12,"-",D12)</f>
+        <v>1-3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>1.5176777777777748</v>
+        <v>1.1198035087719296</v>
       </c>
       <c r="B13" s="3">
-        <v>0.59999999999999942</v>
+        <v>0.32937894736842127</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>2-1</v>
+        <v>1-0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>1.6371104166666632</v>
+        <v>0.69153982300884731</v>
       </c>
       <c r="B14" s="3">
-        <v>1.7399999999999984</v>
+        <v>0.72713864306784659</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>2-2</v>
+        <v>1-1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>1.5622249999999966</v>
+        <v>0.85040707964601492</v>
       </c>
       <c r="B15" s="3">
-        <v>1.1122222222222213</v>
+        <v>1.0372418879056047</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="9"/>
@@ -649,15 +649,15 @@
       </c>
       <c r="E15" s="2" t="str">
         <f t="shared" si="10"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>1.8804560185185144</v>
+        <v>1.5713840707964548</v>
       </c>
       <c r="B16" s="3">
-        <v>0.88888888888888806</v>
+        <v>0.48042477876106182</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" ref="C16:C55" si="11">ROUND(A16,0)</f>
@@ -665,19 +665,19 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" ref="D16:D55" si="12">ROUND(B16,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="2" t="str">
         <f t="shared" ref="E16:E55" si="13">CONCATENATE(C16,"-",D16)</f>
-        <v>2-1</v>
+        <v>2-0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>0.66564814814814677</v>
+        <v>1.2615929203539782</v>
       </c>
       <c r="B17" s="3">
-        <v>1.2133333333333323</v>
+        <v>0.68436578171091444</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="11"/>
@@ -694,34 +694,34 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>0.95392499999999802</v>
+        <v>1.6203545454545443</v>
       </c>
       <c r="B18" s="3">
-        <v>0.36833333333333301</v>
+        <v>1.2057913636363617</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>1-0</v>
+        <v>2-1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>1.6241814814814781</v>
+        <v>1.184261946902651</v>
       </c>
       <c r="B19" s="3">
-        <v>1.1899999999999988</v>
+        <v>0.63055752212389371</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="12"/>
@@ -729,728 +729,325 @@
       </c>
       <c r="E19" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>0.92921921296296084</v>
+        <v>0.81816637168141315</v>
       </c>
       <c r="B20" s="3">
-        <v>1.1716666666666655</v>
+        <v>0.9196165191740413</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="C20:C24" si="14">ROUND(A20,0)</f>
         <v>1</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="D20:D24" si="15">ROUND(B20,0)</f>
         <v>1</v>
       </c>
       <c r="E20" s="2" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="E20:E24" si="16">CONCATENATE(C20,"-",D20)</f>
         <v>1-1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>1.024586111111109</v>
+        <v>1.8529061946902594</v>
       </c>
       <c r="B21" s="3">
-        <v>0.53444444444444394</v>
+        <v>0.60463716814159285</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
+        <f t="shared" si="14"/>
+        <v>2</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="E21" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-1</v>
+        <f t="shared" si="16"/>
+        <v>2-1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>1.3629145833333305</v>
+        <v>1.2858902654867215</v>
       </c>
       <c r="B22" s="3">
-        <v>0.91111111111111021</v>
+        <v>0.49958702064896754</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
       <c r="E22" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-1</v>
+        <f t="shared" si="16"/>
+        <v>1-0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>1.64896822429906</v>
+        <v>2.0045309734513204</v>
       </c>
       <c r="B23" s="3">
-        <v>0.53933457943925356</v>
+        <v>0.9196165191740413</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="E23" s="2" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>2-1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>0.80074766355139904</v>
+        <v>1.3763044247787566</v>
       </c>
       <c r="B24" s="3">
-        <v>1.4812710280373866</v>
+        <v>0.46348672566371679</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
       <c r="E24" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-1</v>
+        <f t="shared" si="16"/>
+        <v>1-0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>1.1339158878504634</v>
-      </c>
-      <c r="B25" s="3">
-        <v>1.1282822429906567</v>
-      </c>
-      <c r="C25" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D25" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E25" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-1</v>
-      </c>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>1.4299065420560699</v>
-      </c>
-      <c r="B26" s="3">
-        <v>1.538242990654209</v>
-      </c>
-      <c r="C26" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D26" s="1">
-        <f t="shared" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="E26" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-2</v>
-      </c>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>1.3584112149532663</v>
-      </c>
-      <c r="B27" s="3">
-        <v>1.146560747663554</v>
-      </c>
-      <c r="C27" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E27" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-1</v>
-      </c>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>0.88296728971962313</v>
-      </c>
-      <c r="B28" s="3">
-        <v>0.50633831775701055</v>
-      </c>
-      <c r="C28" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D28" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E28" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-1</v>
-      </c>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>1.1954018691588746</v>
-      </c>
-      <c r="B29" s="3">
-        <v>0.71143738317757177</v>
-      </c>
-      <c r="C29" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D29" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E29" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-1</v>
-      </c>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>3.2670504672897089</v>
-      </c>
-      <c r="B30" s="3">
-        <v>1.0103028037383202</v>
-      </c>
-      <c r="C30" s="1">
-        <f t="shared" si="11"/>
-        <v>3</v>
-      </c>
-      <c r="D30" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E30" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>3-1</v>
-      </c>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>1.9415271028037318</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1.2313065420560776</v>
-      </c>
-      <c r="C31" s="1">
-        <f t="shared" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="D31" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E31" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>2-1</v>
-      </c>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>1.2658252427184469</v>
-      </c>
-      <c r="B32" s="3">
-        <v>2.1322485436893164</v>
-      </c>
-      <c r="C32" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D32" s="1">
-        <f t="shared" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="E32" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-2</v>
-      </c>
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>3.8931844660194184</v>
-      </c>
-      <c r="B33" s="3">
-        <v>1.1790291262135901</v>
-      </c>
-      <c r="C33" s="1">
-        <f t="shared" si="11"/>
-        <v>4</v>
-      </c>
-      <c r="D33" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E33" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>4-1</v>
-      </c>
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>1.2522407766990296</v>
-      </c>
-      <c r="B34" s="3">
-        <v>0.44982524271844576</v>
-      </c>
-      <c r="C34" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D34" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="E34" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-0</v>
-      </c>
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <v>1.4912038834951458</v>
-      </c>
-      <c r="B35" s="3">
-        <v>0.54786407766990186</v>
-      </c>
-      <c r="C35" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D35" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E35" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-1</v>
-      </c>
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>1.5000029126213597</v>
-      </c>
-      <c r="B36" s="3">
-        <v>0.93194563106795947</v>
-      </c>
-      <c r="C36" s="1">
-        <f t="shared" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="D36" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E36" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>2-1</v>
-      </c>
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <v>0.51386181818181631</v>
-      </c>
-      <c r="B37" s="3">
-        <v>0.38225454545454507</v>
-      </c>
-      <c r="C37" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D37" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="E37" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-0</v>
-      </c>
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>0.53192727272727092</v>
-      </c>
-      <c r="B38" s="3">
-        <v>0.80290909090909024</v>
-      </c>
-      <c r="C38" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D38" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E38" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-1</v>
-      </c>
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
-        <v>1.0572054545454508</v>
-      </c>
-      <c r="B39" s="3">
-        <v>0.52559999999999951</v>
-      </c>
-      <c r="C39" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D39" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E39" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-1</v>
-      </c>
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <v>0.48174545454545276</v>
-      </c>
-      <c r="B40" s="3">
-        <v>3.4379999999999966</v>
-      </c>
-      <c r="C40" s="1">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="D40" s="1">
-        <f t="shared" si="12"/>
-        <v>3</v>
-      </c>
-      <c r="E40" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>0-3</v>
-      </c>
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
-        <v>3.4203927272727146</v>
-      </c>
-      <c r="B41" s="3">
-        <v>0.9599999999999993</v>
-      </c>
-      <c r="C41" s="1">
-        <f t="shared" si="11"/>
-        <v>3</v>
-      </c>
-      <c r="D41" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E41" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>3-1</v>
-      </c>
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
-        <v>0.56649230769230707</v>
-      </c>
-      <c r="B42" s="3">
-        <v>1.0259999999999965</v>
-      </c>
-      <c r="C42" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D42" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E42" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-1</v>
-      </c>
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="2"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
-        <v>6.9569230769230703E-2</v>
-      </c>
-      <c r="B43" s="3">
-        <v>3.3629538461538346</v>
-      </c>
-      <c r="C43" s="1">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="D43" s="1">
-        <f t="shared" si="12"/>
-        <v>3</v>
-      </c>
-      <c r="E43" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>0-3</v>
-      </c>
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
-        <v>0.71556923076922996</v>
-      </c>
-      <c r="B44" s="3">
-        <v>1.901630769230763</v>
-      </c>
-      <c r="C44" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D44" s="1">
-        <f t="shared" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="E44" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-2</v>
-      </c>
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
-        <v>1.9116923076923058</v>
-      </c>
-      <c r="B45" s="3">
-        <v>1.202676923076919</v>
-      </c>
-      <c r="C45" s="1">
-        <f t="shared" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="D45" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E45" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>2-1</v>
-      </c>
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
-        <v>1.641892307692306</v>
-      </c>
-      <c r="B46" s="3">
-        <v>1.4787692307692257</v>
-      </c>
-      <c r="C46" s="1">
-        <f t="shared" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="D46" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E46" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>2-1</v>
-      </c>
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
-        <v>1.4337187878787931</v>
-      </c>
-      <c r="B47" s="3">
-        <v>0.63415757575757536</v>
-      </c>
-      <c r="C47" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D47" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E47" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-1</v>
-      </c>
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
-        <v>1.3431854545454593</v>
-      </c>
-      <c r="B48" s="3">
-        <v>0.88530909090909027</v>
-      </c>
-      <c r="C48" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D48" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E48" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-1</v>
-      </c>
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
-        <v>1.5290727272727327</v>
-      </c>
-      <c r="B49" s="3">
-        <v>0.57646060606060578</v>
-      </c>
-      <c r="C49" s="1">
-        <f t="shared" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="D49" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E49" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>2-1</v>
-      </c>
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
-        <v>1.2952145454545501</v>
-      </c>
-      <c r="B50" s="3">
-        <v>0.94512727272727215</v>
-      </c>
-      <c r="C50" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D50" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E50" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-1</v>
-      </c>
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="2"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="3">
-        <v>0.80351272727273026</v>
-      </c>
-      <c r="B51" s="3">
-        <v>0.48533333333333301</v>
-      </c>
-      <c r="C51" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D51" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="E51" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-0</v>
-      </c>
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="3">
-        <v>0.93966545454545802</v>
-      </c>
-      <c r="B52" s="3">
-        <v>0.34533333333333316</v>
-      </c>
-      <c r="C52" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D52" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="E52" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-0</v>
-      </c>
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="3">
-        <v>0.82373575757576045</v>
-      </c>
-      <c r="B53" s="3">
-        <v>0.26812121212121198</v>
-      </c>
-      <c r="C53" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="D53" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="E53" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>1-0</v>
-      </c>
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="2"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="3">
-        <v>1.7269527272727336</v>
-      </c>
-      <c r="B54" s="3">
-        <v>0.3046909090909089</v>
-      </c>
-      <c r="C54" s="1">
-        <f t="shared" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="D54" s="1">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="E54" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>2-0</v>
-      </c>
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="2"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="3">
-        <v>0.28782545454545561</v>
-      </c>
-      <c r="B55" s="3">
-        <v>0.78756363636363591</v>
-      </c>
-      <c r="C55" s="1">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="D55" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="E55" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>0-1</v>
-      </c>
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="2"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>

</xml_diff>

<commit_message>
updated correct score generators
</commit_message>
<xml_diff>
--- a/CS generator.xlsx
+++ b/CS generator.xlsx
@@ -12,8 +12,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="score" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -85,6 +88,446 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="score_newleagues"/>
+      <sheetName val="cs_lookupnewleagues"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>1-0</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>2-0</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>2-1</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>3-0</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>3-1</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>3-2</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>4-0</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>4-1</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>4-2</v>
+          </cell>
+          <cell r="B10" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>4-3</v>
+          </cell>
+          <cell r="B11" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>5-0</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>5-1</v>
+          </cell>
+          <cell r="B13" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>5-2</v>
+          </cell>
+          <cell r="B14" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>5-3</v>
+          </cell>
+          <cell r="B15" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>5-4</v>
+          </cell>
+          <cell r="B16" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>6-0</v>
+          </cell>
+          <cell r="B17" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>6-1</v>
+          </cell>
+          <cell r="B18" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>6-2</v>
+          </cell>
+          <cell r="B19" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>6-3</v>
+          </cell>
+          <cell r="B20" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>6-4</v>
+          </cell>
+          <cell r="B21" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>6-5</v>
+          </cell>
+          <cell r="B22" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>7-0</v>
+          </cell>
+          <cell r="B23" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24" t="str">
+            <v>7-2</v>
+          </cell>
+          <cell r="B24" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25" t="str">
+            <v>9-0</v>
+          </cell>
+          <cell r="B25" t="str">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26" t="str">
+            <v>0-0</v>
+          </cell>
+          <cell r="B26" t="str">
+            <v>X</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27" t="str">
+            <v>1-1</v>
+          </cell>
+          <cell r="B27" t="str">
+            <v>X</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
+            <v>2-2</v>
+          </cell>
+          <cell r="B28" t="str">
+            <v>X</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29" t="str">
+            <v>3-3</v>
+          </cell>
+          <cell r="B29" t="str">
+            <v>X</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30" t="str">
+            <v>4-4</v>
+          </cell>
+          <cell r="B30" t="str">
+            <v>X</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31" t="str">
+            <v>5-5</v>
+          </cell>
+          <cell r="B31" t="str">
+            <v>X</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32" t="str">
+            <v>0-1</v>
+          </cell>
+          <cell r="B32" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33" t="str">
+            <v>0-2</v>
+          </cell>
+          <cell r="B33" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34" t="str">
+            <v>1-2</v>
+          </cell>
+          <cell r="B34" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35" t="str">
+            <v>0-3</v>
+          </cell>
+          <cell r="B35" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36" t="str">
+            <v>1-3</v>
+          </cell>
+          <cell r="B36" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37" t="str">
+            <v>2-3</v>
+          </cell>
+          <cell r="B37" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38" t="str">
+            <v>0-4</v>
+          </cell>
+          <cell r="B38" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39" t="str">
+            <v>1-4</v>
+          </cell>
+          <cell r="B39" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40" t="str">
+            <v>2-4</v>
+          </cell>
+          <cell r="B40" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41" t="str">
+            <v>3-4</v>
+          </cell>
+          <cell r="B41" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42" t="str">
+            <v>0-5</v>
+          </cell>
+          <cell r="B42" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43" t="str">
+            <v>1-5</v>
+          </cell>
+          <cell r="B43" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44" t="str">
+            <v>2-5</v>
+          </cell>
+          <cell r="B44" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45" t="str">
+            <v>3-5</v>
+          </cell>
+          <cell r="B45" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46" t="str">
+            <v>4-5</v>
+          </cell>
+          <cell r="B46" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47" t="str">
+            <v>0-6</v>
+          </cell>
+          <cell r="B47" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48" t="str">
+            <v>1-6</v>
+          </cell>
+          <cell r="B48" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49" t="str">
+            <v>2-6</v>
+          </cell>
+          <cell r="B49" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50" t="str">
+            <v>3-6</v>
+          </cell>
+          <cell r="B50" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51" t="str">
+            <v>4-6</v>
+          </cell>
+          <cell r="B51" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52" t="str">
+            <v>3-8</v>
+          </cell>
+          <cell r="B52" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53" t="str">
+            <v>5-6</v>
+          </cell>
+          <cell r="B53" t="str">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54" t="str">
+            <v>P</v>
+          </cell>
+          <cell r="B54" t="str">
+            <v>P</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -350,15 +793,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E196"/>
+  <dimension ref="A1:F196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E191"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4">
         <v>1.2919841792</v>
       </c>
@@ -377,8 +820,12 @@
         <f>CONCATENATE(C1,"-",D1)</f>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="5" t="str">
+        <f>VLOOKUP(E1,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>2.2994317317199999</v>
       </c>
@@ -397,8 +844,12 @@
         <f t="shared" ref="E2" si="2">CONCATENATE(C2,"-",D2)</f>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="5" t="str">
+        <f>VLOOKUP(E2,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -406,19 +857,23 @@
         <v>#N/A</v>
       </c>
       <c r="C3" s="1" t="e">
-        <f t="shared" ref="C3:C66" si="3">ROUND(A3,0)</f>
+        <f t="shared" ref="C3:C11" si="3">ROUND(A3,0)</f>
         <v>#N/A</v>
       </c>
       <c r="D3" s="1" t="e">
-        <f t="shared" ref="D3:D66" si="4">ROUND(B3,0)</f>
+        <f t="shared" ref="D3:D11" si="4">ROUND(B3,0)</f>
         <v>#N/A</v>
       </c>
       <c r="E3" s="2" t="e">
-        <f t="shared" ref="E3:E66" si="5">CONCATENATE(C3,"-",D3)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E3:E11" si="5">CONCATENATE(C3,"-",D3)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F3" s="5" t="e">
+        <f>VLOOKUP(E3,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -437,8 +892,12 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="5" t="e">
+        <f>VLOOKUP(E4,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>0.86360097655800017</v>
       </c>
@@ -457,8 +916,12 @@
         <f t="shared" si="5"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="5" t="str">
+        <f>VLOOKUP(E5,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1.3254705629100001</v>
       </c>
@@ -477,8 +940,12 @@
         <f t="shared" si="5"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="5" t="str">
+        <f>VLOOKUP(E6,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>0.83254991707800008</v>
       </c>
@@ -497,8 +964,12 @@
         <f t="shared" si="5"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="5" t="str">
+        <f>VLOOKUP(E7,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>0.59546992389300013</v>
       </c>
@@ -517,8 +988,12 @@
         <f t="shared" si="5"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="5" t="str">
+        <f>VLOOKUP(E8,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>0.579197735298</v>
       </c>
@@ -537,8 +1012,12 @@
         <f t="shared" si="5"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="5" t="str">
+        <f>VLOOKUP(E9,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -557,8 +1036,12 @@
         <f t="shared" si="5"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="5" t="e">
+        <f>VLOOKUP(E10,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>2.0669958221639999</v>
       </c>
@@ -577,8 +1060,12 @@
         <f t="shared" si="5"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="5" t="str">
+        <f>VLOOKUP(E11,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>1.7431916803839997</v>
       </c>
@@ -597,8 +1084,12 @@
         <f t="shared" ref="E12:E75" si="8">CONCATENATE(C12,"-",D12)</f>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="5" t="str">
+        <f>VLOOKUP(E12,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>0.81869183335999995</v>
       </c>
@@ -617,8 +1108,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="5" t="str">
+        <f>VLOOKUP(E13,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -637,8 +1132,12 @@
         <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="5" t="e">
+        <f>VLOOKUP(E14,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>1.4773193499999999</v>
       </c>
@@ -657,8 +1156,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="5" t="str">
+        <f>VLOOKUP(E15,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>1.1696702921640001</v>
       </c>
@@ -677,8 +1180,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="5" t="str">
+        <f>VLOOKUP(E16,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>2.202463281744</v>
       </c>
@@ -697,8 +1204,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="5" t="str">
+        <f>VLOOKUP(E17,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>1.9076710751999999</v>
       </c>
@@ -717,8 +1228,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="5" t="str">
+        <f>VLOOKUP(E18,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>0.65152759077</v>
       </c>
@@ -737,8 +1252,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="5" t="str">
+        <f>VLOOKUP(E19,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>1.5549860731679999</v>
       </c>
@@ -757,8 +1276,12 @@
         <f t="shared" si="8"/>
         <v>2-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="5" t="str">
+        <f>VLOOKUP(E20,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -777,8 +1300,12 @@
         <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="5" t="e">
+        <f>VLOOKUP(E21,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>1.4131429884</v>
       </c>
@@ -797,8 +1324,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="5" t="str">
+        <f>VLOOKUP(E22,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>1.7945969758499998</v>
       </c>
@@ -817,8 +1348,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="5" t="str">
+        <f>VLOOKUP(E23,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -837,8 +1372,12 @@
         <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="5" t="e">
+        <f>VLOOKUP(E24,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -857,8 +1396,12 @@
         <f t="shared" si="8"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="5" t="e">
+        <f>VLOOKUP(E25,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>0.62041928867100005</v>
       </c>
@@ -877,8 +1420,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="5" t="str">
+        <f>VLOOKUP(E26,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>0.81162434566199992</v>
       </c>
@@ -897,8 +1444,12 @@
         <f t="shared" si="8"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="5" t="str">
+        <f>VLOOKUP(E27,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>0.87486026281600004</v>
       </c>
@@ -917,8 +1468,12 @@
         <f t="shared" si="8"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="5" t="str">
+        <f>VLOOKUP(E28,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>0.62140761091499996</v>
       </c>
@@ -937,8 +1492,12 @@
         <f t="shared" si="8"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="5" t="str">
+        <f>VLOOKUP(E29,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>1.2826952083679999</v>
       </c>
@@ -957,8 +1516,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="5" t="str">
+        <f>VLOOKUP(E30,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>2.7192569020820003</v>
       </c>
@@ -977,8 +1540,12 @@
         <f t="shared" si="8"/>
         <v>3-1</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="5" t="str">
+        <f>VLOOKUP(E31,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>1.7773802002530001</v>
       </c>
@@ -997,8 +1564,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="5" t="str">
+        <f>VLOOKUP(E32,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>1.6570065427999998</v>
       </c>
@@ -1017,8 +1588,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="5" t="str">
+        <f>VLOOKUP(E33,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>1.6378326791819999</v>
       </c>
@@ -1037,8 +1612,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="5" t="str">
+        <f>VLOOKUP(E34,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>0.5456906086240001</v>
       </c>
@@ -1057,8 +1636,12 @@
         <f t="shared" si="8"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="5" t="str">
+        <f>VLOOKUP(E35,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>1.5851244921280001</v>
       </c>
@@ -1077,8 +1660,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="5" t="str">
+        <f>VLOOKUP(E36,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>1.1662258411440001</v>
       </c>
@@ -1097,8 +1684,12 @@
         <f t="shared" si="8"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="5" t="str">
+        <f>VLOOKUP(E37,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>0.90112514125199994</v>
       </c>
@@ -1117,8 +1708,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="5" t="str">
+        <f>VLOOKUP(E38,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>2.2896494127440001</v>
       </c>
@@ -1137,8 +1732,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="5" t="str">
+        <f>VLOOKUP(E39,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>1.4258429112720001</v>
       </c>
@@ -1157,8 +1756,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="5" t="str">
+        <f>VLOOKUP(E40,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>2.2282726989600001</v>
       </c>
@@ -1177,8 +1780,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="5" t="str">
+        <f>VLOOKUP(E41,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>1.0690021975360002</v>
       </c>
@@ -1197,8 +1804,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="5" t="str">
+        <f>VLOOKUP(E42,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>2.1231466599640001</v>
       </c>
@@ -1217,8 +1828,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="5" t="str">
+        <f>VLOOKUP(E43,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>0.63430481052400001</v>
       </c>
@@ -1237,8 +1852,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="5" t="str">
+        <f>VLOOKUP(E44,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>1.08732750016</v>
       </c>
@@ -1257,8 +1876,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="5" t="str">
+        <f>VLOOKUP(E45,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>0.36543386809600004</v>
       </c>
@@ -1277,8 +1900,12 @@
         <f t="shared" si="8"/>
         <v>0-1</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="5" t="str">
+        <f>VLOOKUP(E46,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>1.1416547439000002</v>
       </c>
@@ -1297,8 +1924,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" s="5" t="str">
+        <f>VLOOKUP(E47,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>0.98739534227400005</v>
       </c>
@@ -1317,8 +1948,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="5" t="str">
+        <f>VLOOKUP(E48,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>1.5225826663519999</v>
       </c>
@@ -1337,8 +1972,12 @@
         <f t="shared" si="8"/>
         <v>2-0</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="5" t="str">
+        <f>VLOOKUP(E49,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>1.1778511668</v>
       </c>
@@ -1357,8 +1996,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="5" t="str">
+        <f>VLOOKUP(E50,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>0.63956144419200001</v>
       </c>
@@ -1377,8 +2020,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" s="5" t="str">
+        <f>VLOOKUP(E51,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>0.72935466049600006</v>
       </c>
@@ -1397,8 +2044,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" s="5" t="str">
+        <f>VLOOKUP(E52,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>1.8845879543920001</v>
       </c>
@@ -1417,8 +2068,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53" s="5" t="str">
+        <f>VLOOKUP(E53,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>3.0232181116499999</v>
       </c>
@@ -1437,8 +2092,12 @@
         <f t="shared" si="8"/>
         <v>3-1</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" s="5" t="str">
+        <f>VLOOKUP(E54,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>1.3741862849400002</v>
       </c>
@@ -1457,8 +2116,12 @@
         <f t="shared" si="8"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" s="5" t="str">
+        <f>VLOOKUP(E55,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>1.2980924621000001</v>
       </c>
@@ -1477,8 +2140,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" s="5" t="str">
+        <f>VLOOKUP(E56,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>1.5652001400000002</v>
       </c>
@@ -1497,8 +2164,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" s="5" t="str">
+        <f>VLOOKUP(E57,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>1.4727772484300001</v>
       </c>
@@ -1517,8 +2188,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" s="5" t="str">
+        <f>VLOOKUP(E58,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>1.5652001400000002</v>
       </c>
@@ -1537,8 +2212,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59" s="5" t="str">
+        <f>VLOOKUP(E59,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>2.6988353399880003</v>
       </c>
@@ -1557,8 +2236,12 @@
         <f t="shared" si="8"/>
         <v>3-1</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60" s="5" t="str">
+        <f>VLOOKUP(E60,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>1.0940444645360001</v>
       </c>
@@ -1577,8 +2260,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61" s="5" t="str">
+        <f>VLOOKUP(E61,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>1.2608669000000001</v>
       </c>
@@ -1597,8 +2284,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" s="5" t="str">
+        <f>VLOOKUP(E62,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>1.178134838688</v>
       </c>
@@ -1617,8 +2308,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63" s="5" t="str">
+        <f>VLOOKUP(E63,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>1.9812595305600003</v>
       </c>
@@ -1637,8 +2332,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" s="5" t="str">
+        <f>VLOOKUP(E64,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>0.98457827805999998</v>
       </c>
@@ -1657,8 +2356,12 @@
         <f t="shared" si="8"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" s="5" t="str">
+        <f>VLOOKUP(E65,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>1.7054274201479998</v>
       </c>
@@ -1677,8 +2380,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" s="5" t="str">
+        <f>VLOOKUP(E66,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>1.7252008287299998</v>
       </c>
@@ -1697,8 +2404,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F67" s="5" t="str">
+        <f>VLOOKUP(E67,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>1.4871360494339998</v>
       </c>
@@ -1717,8 +2428,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F68" s="5" t="str">
+        <f>VLOOKUP(E68,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>1.0795223089799999</v>
       </c>
@@ -1737,8 +2452,12 @@
         <f t="shared" si="8"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" s="5" t="str">
+        <f>VLOOKUP(E69,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>1.2554187416099998</v>
       </c>
@@ -1757,8 +2476,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" s="5" t="str">
+        <f>VLOOKUP(E70,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>1.6311332251439998</v>
       </c>
@@ -1777,8 +2500,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71" s="5" t="str">
+        <f>VLOOKUP(E71,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>1.3491637565399999</v>
       </c>
@@ -1797,8 +2524,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72" s="5" t="str">
+        <f>VLOOKUP(E72,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>0.92351884347000002</v>
       </c>
@@ -1817,8 +2548,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" s="5" t="str">
+        <f>VLOOKUP(E73,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>2.4102087360479998</v>
       </c>
@@ -1837,8 +2572,12 @@
         <f t="shared" si="8"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" s="5" t="str">
+        <f>VLOOKUP(E74,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>0.84159955745999993</v>
       </c>
@@ -1857,8 +2596,12 @@
         <f t="shared" si="8"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75" s="5" t="str">
+        <f>VLOOKUP(E75,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>0.62961699902399992</v>
       </c>
@@ -1877,8 +2620,12 @@
         <f t="shared" ref="E76:E139" si="11">CONCATENATE(C76,"-",D76)</f>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" s="5" t="str">
+        <f>VLOOKUP(E76,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>1.1982582631320002</v>
       </c>
@@ -1897,8 +2644,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77" s="5" t="str">
+        <f>VLOOKUP(E77,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>2.4330055412880003</v>
       </c>
@@ -1917,8 +2668,12 @@
         <f t="shared" si="11"/>
         <v>2-0</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78" s="5" t="str">
+        <f>VLOOKUP(E78,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>1.0743178844160002</v>
       </c>
@@ -1937,8 +2692,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79" s="5" t="str">
+        <f>VLOOKUP(E79,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>1.0330071235680001</v>
       </c>
@@ -1957,8 +2716,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80" s="5" t="str">
+        <f>VLOOKUP(E80,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>2.8098550917360003</v>
       </c>
@@ -1977,8 +2740,12 @@
         <f t="shared" si="11"/>
         <v>3-1</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81" s="5" t="str">
+        <f>VLOOKUP(E81,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>1.0361854329119999</v>
       </c>
@@ -1997,8 +2764,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82" s="5" t="str">
+        <f>VLOOKUP(E82,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>2.8712920718160007</v>
       </c>
@@ -2017,8 +2788,12 @@
         <f t="shared" si="11"/>
         <v>3-1</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83" s="5" t="str">
+        <f>VLOOKUP(E83,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>0.99163183824600021</v>
       </c>
@@ -2037,8 +2812,12 @@
         <f t="shared" si="11"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84" s="5" t="str">
+        <f>VLOOKUP(E84,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>3.1575499810680001</v>
       </c>
@@ -2057,8 +2836,12 @@
         <f t="shared" si="11"/>
         <v>3-1</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85" s="5" t="str">
+        <f>VLOOKUP(E85,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>0.441340789806</v>
       </c>
@@ -2077,8 +2860,12 @@
         <f t="shared" si="11"/>
         <v>0-2</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86" s="5" t="str">
+        <f>VLOOKUP(E86,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>1.734476803488</v>
       </c>
@@ -2097,8 +2884,12 @@
         <f t="shared" si="11"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87" s="5" t="str">
+        <f>VLOOKUP(E87,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>1.585792325568</v>
       </c>
@@ -2117,8 +2908,12 @@
         <f t="shared" si="11"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88" s="5" t="str">
+        <f>VLOOKUP(E88,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>1.3083152687640001</v>
       </c>
@@ -2137,8 +2932,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89" s="5" t="str">
+        <f>VLOOKUP(E89,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>3.26302185706</v>
       </c>
@@ -2157,8 +2956,12 @@
         <f t="shared" si="11"/>
         <v>3-1</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90" s="5" t="str">
+        <f>VLOOKUP(E90,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -2177,8 +2980,12 @@
         <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91" s="5" t="e">
+        <f>VLOOKUP(E91,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>1.0176543296640002</v>
       </c>
@@ -2197,8 +3004,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92" s="5" t="str">
+        <f>VLOOKUP(E92,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>1.4419731103050002</v>
       </c>
@@ -2217,8 +3028,12 @@
         <f t="shared" si="11"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F93" s="5" t="str">
+        <f>VLOOKUP(E93,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>0.98057118814200006</v>
       </c>
@@ -2237,8 +3052,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F94" s="5" t="str">
+        <f>VLOOKUP(E94,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>2.1646193143680001</v>
       </c>
@@ -2257,8 +3076,12 @@
         <f t="shared" si="11"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F95" s="5" t="str">
+        <f>VLOOKUP(E95,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -2277,8 +3100,12 @@
         <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F96" s="5" t="e">
+        <f>VLOOKUP(E96,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>1.3740373467939999</v>
       </c>
@@ -2297,8 +3124,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F97" s="5" t="str">
+        <f>VLOOKUP(E97,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>1.038233268842</v>
       </c>
@@ -2317,8 +3148,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F98" s="5" t="str">
+        <f>VLOOKUP(E98,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>2.6707984608240003</v>
       </c>
@@ -2337,8 +3172,12 @@
         <f t="shared" si="11"/>
         <v>3-1</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99" s="5" t="str">
+        <f>VLOOKUP(E99,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>2.3914297682730004</v>
       </c>
@@ -2357,8 +3196,12 @@
         <f t="shared" si="11"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100" s="5" t="str">
+        <f>VLOOKUP(E100,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>1.4053164044400004</v>
       </c>
@@ -2377,8 +3220,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F101" s="5" t="str">
+        <f>VLOOKUP(E101,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>1.7012487673350001</v>
       </c>
@@ -2397,8 +3244,12 @@
         <f t="shared" si="11"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F102" s="5" t="str">
+        <f>VLOOKUP(E102,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>0.98246214729000003</v>
       </c>
@@ -2417,8 +3268,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F103" s="5" t="str">
+        <f>VLOOKUP(E103,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -2437,8 +3292,12 @@
         <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F104" s="5" t="e">
+        <f>VLOOKUP(E104,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -2457,8 +3316,12 @@
         <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F105" s="5" t="e">
+        <f>VLOOKUP(E105,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -2477,8 +3340,12 @@
         <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F106" s="5" t="e">
+        <f>VLOOKUP(E106,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>2.0145105189420001</v>
       </c>
@@ -2497,8 +3364,12 @@
         <f t="shared" si="11"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F107" s="5" t="str">
+        <f>VLOOKUP(E107,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>1.6571183807099998</v>
       </c>
@@ -2517,8 +3388,12 @@
         <f t="shared" si="11"/>
         <v>2-2</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F108" s="5" t="str">
+        <f>VLOOKUP(E108,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -2537,8 +3412,12 @@
         <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F109" s="5" t="e">
+        <f>VLOOKUP(E109,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -2557,8 +3436,12 @@
         <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F110" s="5" t="e">
+        <f>VLOOKUP(E110,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>0.51846169127999997</v>
       </c>
@@ -2577,8 +3460,12 @@
         <f t="shared" si="11"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F111" s="5" t="str">
+        <f>VLOOKUP(E111,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>0.43934085000000006</v>
       </c>
@@ -2597,8 +3484,12 @@
         <f t="shared" si="11"/>
         <v>0-1</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F112" s="5" t="str">
+        <f>VLOOKUP(E112,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>1.330954092</v>
       </c>
@@ -2617,8 +3508,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F113" s="5" t="str">
+        <f>VLOOKUP(E113,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>1.1170814654999999</v>
       </c>
@@ -2637,8 +3532,12 @@
         <f t="shared" si="11"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F114" s="5" t="str">
+        <f>VLOOKUP(E114,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>1.9590004793640001</v>
       </c>
@@ -2657,8 +3556,12 @@
         <f t="shared" si="11"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F115" s="5" t="str">
+        <f>VLOOKUP(E115,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>1.6015928151850001</v>
       </c>
@@ -2677,8 +3580,12 @@
         <f t="shared" si="11"/>
         <v>2-2</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F116" s="5" t="str">
+        <f>VLOOKUP(E116,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>1.6375868213489999</v>
       </c>
@@ -2697,8 +3604,12 @@
         <f t="shared" si="11"/>
         <v>2-0</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F117" s="5" t="str">
+        <f>VLOOKUP(E117,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>2.0633883824530002</v>
       </c>
@@ -2717,8 +3628,12 @@
         <f t="shared" si="11"/>
         <v>2-2</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F118" s="5" t="str">
+        <f>VLOOKUP(E118,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>0.70374677072699998</v>
       </c>
@@ -2737,8 +3652,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F119" s="5" t="str">
+        <f>VLOOKUP(E119,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>1.5835325030910001</v>
       </c>
@@ -2757,8 +3676,12 @@
         <f t="shared" si="11"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F120" s="5" t="str">
+        <f>VLOOKUP(E120,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>0.70711163107199992</v>
       </c>
@@ -2777,8 +3700,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F121" s="5" t="str">
+        <f>VLOOKUP(E121,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>1.448665357986</v>
       </c>
@@ -2797,8 +3724,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F122" s="5" t="str">
+        <f>VLOOKUP(E122,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>0.51136718749999999</v>
       </c>
@@ -2817,8 +3748,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F123" s="5" t="str">
+        <f>VLOOKUP(E123,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>0.70383127895599995</v>
       </c>
@@ -2837,8 +3772,12 @@
         <f t="shared" si="11"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F124" s="5" t="str">
+        <f>VLOOKUP(E124,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -2857,8 +3796,12 @@
         <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F125" s="5" t="e">
+        <f>VLOOKUP(E125,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>1.2500268624999999</v>
       </c>
@@ -2877,8 +3820,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F126" s="5" t="str">
+        <f>VLOOKUP(E126,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>1.396780533896</v>
       </c>
@@ -2897,8 +3844,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F127" s="5" t="str">
+        <f>VLOOKUP(E127,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>0.80164191738400004</v>
       </c>
@@ -2917,8 +3868,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F128" s="5" t="str">
+        <f>VLOOKUP(E128,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>1.8583507621800002</v>
       </c>
@@ -2937,8 +3892,12 @@
         <f t="shared" si="11"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F129" s="5" t="str">
+        <f>VLOOKUP(E129,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>0.81982301345999997</v>
       </c>
@@ -2957,8 +3916,12 @@
         <f t="shared" si="11"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F130" s="5" t="str">
+        <f>VLOOKUP(E130,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>1.0304711566079998</v>
       </c>
@@ -2977,8 +3940,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F131" s="5" t="str">
+        <f>VLOOKUP(E131,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -2997,8 +3964,12 @@
         <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F132" s="5" t="e">
+        <f>VLOOKUP(E132,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>1.1152975721039999</v>
       </c>
@@ -3017,8 +3988,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F133" s="5" t="str">
+        <f>VLOOKUP(E133,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>1.224302221608</v>
       </c>
@@ -3037,8 +4012,12 @@
         <f t="shared" si="11"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F134" s="5" t="str">
+        <f>VLOOKUP(E134,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>1.166227057512</v>
       </c>
@@ -3057,8 +4036,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F135" s="5" t="str">
+        <f>VLOOKUP(E135,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>1.166227057512</v>
       </c>
@@ -3077,8 +4060,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F136" s="5" t="str">
+        <f>VLOOKUP(E136,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>2.605047656904</v>
       </c>
@@ -3097,8 +4084,12 @@
         <f t="shared" si="11"/>
         <v>3-1</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F137" s="5" t="str">
+        <f>VLOOKUP(E137,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>1.3953957130079999</v>
       </c>
@@ -3117,8 +4108,12 @@
         <f t="shared" si="11"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F138" s="5" t="str">
+        <f>VLOOKUP(E138,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>0.71560438962500006</v>
       </c>
@@ -3137,8 +4132,12 @@
         <f t="shared" si="11"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F139" s="5" t="str">
+        <f>VLOOKUP(E139,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>2.4228585678249996</v>
       </c>
@@ -3157,8 +4156,12 @@
         <f t="shared" ref="E140:E191" si="14">CONCATENATE(C140,"-",D140)</f>
         <v>2-2</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F140" s="5" t="str">
+        <f>VLOOKUP(E140,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>1.9605261534249998</v>
       </c>
@@ -3177,8 +4180,12 @@
         <f t="shared" si="14"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F141" s="5" t="str">
+        <f>VLOOKUP(E141,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>2.2949294947499999</v>
       </c>
@@ -3197,8 +4204,12 @@
         <f t="shared" si="14"/>
         <v>2-2</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F142" s="5" t="str">
+        <f>VLOOKUP(E142,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>2.0288902831660001</v>
       </c>
@@ -3217,8 +4228,12 @@
         <f t="shared" si="14"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F143" s="5" t="str">
+        <f>VLOOKUP(E143,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>0.8816658018350001</v>
       </c>
@@ -3237,8 +4252,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F144" s="5" t="str">
+        <f>VLOOKUP(E144,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -3257,8 +4276,12 @@
         <f t="shared" si="14"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F145" s="5" t="e">
+        <f>VLOOKUP(E145,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>1.7161382872199999</v>
       </c>
@@ -3277,8 +4300,12 @@
         <f t="shared" si="14"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F146" s="5" t="str">
+        <f>VLOOKUP(E146,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -3297,8 +4324,12 @@
         <f t="shared" si="14"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F147" s="5" t="e">
+        <f>VLOOKUP(E147,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>0.946248769968</v>
       </c>
@@ -3317,8 +4348,12 @@
         <f t="shared" si="14"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F148" s="5" t="str">
+        <f>VLOOKUP(E148,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>1.151684633688</v>
       </c>
@@ -3337,8 +4372,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F149" s="5" t="str">
+        <f>VLOOKUP(E149,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>0.68810340979600004</v>
       </c>
@@ -3357,8 +4396,12 @@
         <f t="shared" si="14"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F150" s="5" t="str">
+        <f>VLOOKUP(E150,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>1.3842675841500001</v>
       </c>
@@ -3377,8 +4420,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F151" s="5" t="str">
+        <f>VLOOKUP(E151,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>0.75328451215199999</v>
       </c>
@@ -3397,8 +4444,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F152" s="5" t="str">
+        <f>VLOOKUP(E152,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>1.676849983848</v>
       </c>
@@ -3417,8 +4468,12 @@
         <f t="shared" si="14"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F153" s="5" t="str">
+        <f>VLOOKUP(E153,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>2.164715050956</v>
       </c>
@@ -3437,8 +4492,12 @@
         <f t="shared" si="14"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F154" s="5" t="str">
+        <f>VLOOKUP(E154,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>1.3736576290140001</v>
       </c>
@@ -3457,8 +4516,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F155" s="5" t="str">
+        <f>VLOOKUP(E155,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>1.4986035368759998</v>
       </c>
@@ -3477,8 +4540,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F156" s="5" t="str">
+        <f>VLOOKUP(E156,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>0.44402521945200002</v>
       </c>
@@ -3497,8 +4564,12 @@
         <f t="shared" si="14"/>
         <v>0-2</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F157" s="5" t="str">
+        <f>VLOOKUP(E157,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>1.0372616209800001</v>
       </c>
@@ -3517,8 +4588,12 @@
         <f t="shared" si="14"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F158" s="5" t="str">
+        <f>VLOOKUP(E158,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>1.4784690697920002</v>
       </c>
@@ -3537,8 +4612,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F159" s="5" t="str">
+        <f>VLOOKUP(E159,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>1.4256083350080002</v>
       </c>
@@ -3557,8 +4636,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F160" s="5" t="str">
+        <f>VLOOKUP(E160,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>2.0456718668100002</v>
       </c>
@@ -3577,8 +4660,12 @@
         <f t="shared" si="14"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F161" s="5" t="str">
+        <f>VLOOKUP(E161,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
         <v>2.4271755728219997</v>
       </c>
@@ -3597,8 +4684,12 @@
         <f t="shared" si="14"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F162" s="5" t="str">
+        <f>VLOOKUP(E162,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="e">
         <v>#N/A</v>
       </c>
@@ -3617,8 +4708,12 @@
         <f t="shared" si="14"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F163" s="5" t="e">
+        <f>VLOOKUP(E163,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>1.2631325356259999</v>
       </c>
@@ -3637,8 +4732,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F164" s="5" t="str">
+        <f>VLOOKUP(E164,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>0.78584396482800001</v>
       </c>
@@ -3657,8 +4756,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F165" s="5" t="str">
+        <f>VLOOKUP(E165,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="e">
         <v>#N/A</v>
       </c>
@@ -3677,8 +4780,12 @@
         <f t="shared" si="14"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F166" s="5" t="e">
+        <f>VLOOKUP(E166,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>1.063262633706</v>
       </c>
@@ -3697,8 +4804,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F167" s="5" t="str">
+        <f>VLOOKUP(E167,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>1.3364575428599998</v>
       </c>
@@ -3717,8 +4828,12 @@
         <f t="shared" si="14"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F168" s="5" t="str">
+        <f>VLOOKUP(E168,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>3.7771211916480003</v>
       </c>
@@ -3737,8 +4852,12 @@
         <f t="shared" si="14"/>
         <v>4-1</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F169" s="5" t="str">
+        <f>VLOOKUP(E169,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="e">
         <v>#N/A</v>
       </c>
@@ -3757,8 +4876,12 @@
         <f t="shared" si="14"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F170" s="5" t="e">
+        <f>VLOOKUP(E170,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>0.42615312984599996</v>
       </c>
@@ -3777,8 +4900,12 @@
         <f t="shared" si="14"/>
         <v>0-2</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F171" s="5" t="str">
+        <f>VLOOKUP(E171,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>3.04544538708</v>
       </c>
@@ -3797,8 +4924,12 @@
         <f t="shared" si="14"/>
         <v>3-1</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F172" s="5" t="str">
+        <f>VLOOKUP(E172,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>1.25253085648</v>
       </c>
@@ -3817,8 +4948,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F173" s="5" t="str">
+        <f>VLOOKUP(E173,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>1.2006852782399999</v>
       </c>
@@ -3837,8 +4972,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F174" s="5" t="str">
+        <f>VLOOKUP(E174,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>1.5609685089599998</v>
       </c>
@@ -3857,8 +4996,12 @@
         <f t="shared" si="14"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F175" s="5" t="str">
+        <f>VLOOKUP(E175,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>2.2422341935499999</v>
       </c>
@@ -3877,8 +5020,12 @@
         <f t="shared" si="14"/>
         <v>2-0</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F176" s="5" t="str">
+        <f>VLOOKUP(E176,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>1.5582704825999998</v>
       </c>
@@ -3897,8 +5044,12 @@
         <f t="shared" si="14"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F177" s="5" t="str">
+        <f>VLOOKUP(E177,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>1.0162775453999999</v>
       </c>
@@ -3917,8 +5068,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F178" s="5" t="str">
+        <f>VLOOKUP(E178,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>2.6721362169480001</v>
       </c>
@@ -3937,8 +5092,12 @@
         <f t="shared" si="14"/>
         <v>3-1</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F179" s="5" t="str">
+        <f>VLOOKUP(E179,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>0.86043656441600014</v>
       </c>
@@ -3957,8 +5116,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F180" s="5" t="str">
+        <f>VLOOKUP(E180,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>2.778974088</v>
       </c>
@@ -3977,8 +5140,12 @@
         <f t="shared" si="14"/>
         <v>3-1</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F181" s="5" t="str">
+        <f>VLOOKUP(E181,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>1.7428792586919999</v>
       </c>
@@ -3997,8 +5164,12 @@
         <f t="shared" si="14"/>
         <v>2-1</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F182" s="5" t="str">
+        <f>VLOOKUP(E182,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="e">
         <v>#N/A</v>
       </c>
@@ -4017,8 +5188,12 @@
         <f t="shared" si="14"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F183" s="5" t="e">
+        <f>VLOOKUP(E183,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>0.93467523554999987</v>
       </c>
@@ -4037,8 +5212,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F184" s="5" t="str">
+        <f>VLOOKUP(E184,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="e">
         <v>#N/A</v>
       </c>
@@ -4057,8 +5236,12 @@
         <f t="shared" si="14"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F185" s="5" t="e">
+        <f>VLOOKUP(E185,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="e">
         <v>#N/A</v>
       </c>
@@ -4077,8 +5260,12 @@
         <f t="shared" si="14"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F186" s="5" t="e">
+        <f>VLOOKUP(E186,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>0.82068792933599999</v>
       </c>
@@ -4097,8 +5284,12 @@
         <f t="shared" si="14"/>
         <v>1-2</v>
       </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F187" s="5" t="str">
+        <f>VLOOKUP(E187,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>1.0101139891919999</v>
       </c>
@@ -4117,8 +5308,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F188" s="5" t="str">
+        <f>VLOOKUP(E188,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="e">
         <v>#N/A</v>
       </c>
@@ -4137,8 +5332,12 @@
         <f t="shared" si="14"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F189" s="5" t="e">
+        <f>VLOOKUP(E189,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="e">
         <v>#N/A</v>
       </c>
@@ -4157,8 +5356,12 @@
         <f t="shared" si="14"/>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F190" s="5" t="e">
+        <f>VLOOKUP(E190,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>1.1496410433839999</v>
       </c>
@@ -4177,8 +5380,12 @@
         <f t="shared" si="14"/>
         <v>1-1</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F191" s="5" t="str">
+        <f>VLOOKUP(E191,[1]cs_lookupnewleagues!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C192" s="1"/>
       <c r="D192" s="1"/>
       <c r="E192" s="2"/>

</xml_diff>

<commit_message>
updated fixtures and odds
</commit_message>
<xml_diff>
--- a/CS generator.xlsx
+++ b/CS generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kovan\FDAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22BF326-9725-422B-B6E3-D609592EBC60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6499C124-FE54-4EE6-9E1A-775F951C4D80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -551,29 +551,29 @@
   <dimension ref="A1:J200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E23"/>
+      <selection activeCell="C2" sqref="C2:J65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
-        <v>0.92645532460799995</v>
+        <v>2.5230645010799999</v>
       </c>
       <c r="B1" s="2">
-        <v>0.32118607627199997</v>
+        <v>1.1184931555199999</v>
       </c>
       <c r="C1" s="4">
         <f>ROUND(A1,0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1" s="4">
         <f>ROUND(B1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1" s="5" t="str">
         <f>CONCATENATE(C1,"-",D1)</f>
-        <v>1-0</v>
+        <v>3-1</v>
       </c>
       <c r="F1" s="3" t="str">
         <f>VLOOKUP(E1,cs_lookup!$A$2:$B$54,2,FALSE)</f>
@@ -581,35 +581,35 @@
       </c>
       <c r="H1" s="2">
         <f>ROUND(A1,2)</f>
-        <v>0.93</v>
+        <v>2.52</v>
       </c>
       <c r="I1" s="2">
         <f>ROUND(B1,2)</f>
-        <v>0.32</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="J1" s="2">
         <f>SUM(H1:I1)</f>
-        <v>1.25</v>
+        <v>3.64</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1.5979676564799998</v>
+        <v>1.1556708768000001</v>
       </c>
       <c r="B2" s="1">
-        <v>1.5571890694359998</v>
+        <v>0.70253525472000011</v>
       </c>
       <c r="C2" s="4">
         <f t="shared" ref="C2" si="0">ROUND(A2,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="4">
         <f t="shared" ref="D2" si="1">ROUND(B2,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="5" t="str">
         <f t="shared" ref="E2" si="2">CONCATENATE(C2,"-",D2)</f>
-        <v>2-2</v>
+        <v>1-1</v>
       </c>
       <c r="F2" s="3" t="str">
         <f>VLOOKUP(E2,cs_lookup!$A$2:$B$54,2,FALSE)</f>
@@ -617,63 +617,63 @@
       </c>
       <c r="H2" s="2">
         <f>ROUND(A2,2)</f>
-        <v>1.6</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="I2" s="2">
         <f>ROUND(B2,2)</f>
-        <v>1.56</v>
+        <v>0.7</v>
       </c>
       <c r="J2" s="2">
-        <f t="shared" ref="J2:J65" si="3">SUM(H2:I2)</f>
-        <v>3.16</v>
+        <f t="shared" ref="J2" si="3">SUM(H2:I2)</f>
+        <v>1.8599999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1.1761086753849999</v>
+        <v>2.4395229600000006</v>
       </c>
       <c r="B3" s="1">
-        <v>0.37558267021000002</v>
+        <v>1.5328932849600001</v>
       </c>
       <c r="C3" s="4">
-        <f t="shared" ref="C3:C23" si="4">ROUND(A3,0)</f>
-        <v>1</v>
+        <f t="shared" ref="C3:C65" si="4">ROUND(A3,0)</f>
+        <v>2</v>
       </c>
       <c r="D3" s="4">
-        <f t="shared" ref="D3:D23" si="5">ROUND(B3,0)</f>
-        <v>0</v>
+        <f t="shared" ref="D3:D65" si="5">ROUND(B3,0)</f>
+        <v>2</v>
       </c>
       <c r="E3" s="5" t="str">
-        <f t="shared" ref="E3:E23" si="6">CONCATENATE(C3,"-",D3)</f>
-        <v>1-0</v>
+        <f t="shared" ref="E3:E65" si="6">CONCATENATE(C3,"-",D3)</f>
+        <v>2-2</v>
       </c>
       <c r="F3" s="3" t="str">
         <f>VLOOKUP(E3,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H23" si="7">ROUND(A3,2)</f>
-        <v>1.18</v>
+        <f t="shared" ref="H3:H65" si="7">ROUND(A3,2)</f>
+        <v>2.44</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I23" si="8">ROUND(B3,2)</f>
-        <v>0.38</v>
+        <f t="shared" ref="I3:I65" si="8">ROUND(B3,2)</f>
+        <v>1.53</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J23" si="9">SUM(H3:I3)</f>
-        <v>1.56</v>
+        <f t="shared" ref="J3:J65" si="9">SUM(H3:I3)</f>
+        <v>3.9699999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>0.42336912355500006</v>
+        <v>1.3594133854800001</v>
       </c>
       <c r="B4" s="1">
-        <v>1.3770327554500001</v>
+        <v>1.10390540416</v>
       </c>
       <c r="C4" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" si="5"/>
@@ -681,31 +681,31 @@
       </c>
       <c r="E4" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>0-1</v>
+        <v>1-1</v>
       </c>
       <c r="F4" s="3" t="str">
         <f>VLOOKUP(E4,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="7"/>
-        <v>0.42</v>
+        <v>1.36</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" si="8"/>
-        <v>1.38</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="9"/>
-        <v>1.7999999999999998</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>0.84678824641600003</v>
+        <v>0.90631558836000004</v>
       </c>
       <c r="B5" s="1">
-        <v>0.76302863542400001</v>
+        <v>1.4598859849600001</v>
       </c>
       <c r="C5" s="4">
         <f t="shared" si="4"/>
@@ -725,23 +725,23 @@
       </c>
       <c r="H5" s="2">
         <f t="shared" si="7"/>
-        <v>0.85</v>
+        <v>0.91</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="8"/>
-        <v>0.76</v>
+        <v>1.46</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="9"/>
-        <v>1.6099999999999999</v>
+        <v>2.37</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>0.84213957027899988</v>
+        <v>0.83081428975999994</v>
       </c>
       <c r="B6" s="1">
-        <v>0.43953091036800002</v>
+        <v>0.82119211648000012</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="4"/>
@@ -749,35 +749,35 @@
       </c>
       <c r="D6" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-0</v>
+        <v>1-1</v>
       </c>
       <c r="F6" s="3" t="str">
         <f>VLOOKUP(E6,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" si="7"/>
-        <v>0.84</v>
+        <v>0.83</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" si="8"/>
-        <v>0.44</v>
+        <v>0.82</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="9"/>
-        <v>1.28</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>2.1745154951520003</v>
+        <v>1.5710930225999999</v>
       </c>
       <c r="B7" s="1">
-        <v>0.85842388068800002</v>
+        <v>0.83028802872000007</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="4"/>
@@ -797,35 +797,35 @@
       </c>
       <c r="H7" s="2">
         <f t="shared" si="7"/>
-        <v>2.17</v>
+        <v>1.57</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="8"/>
-        <v>0.86</v>
+        <v>0.83</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="9"/>
-        <v>3.03</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>0.94088694030799991</v>
+        <v>2.9538841436799999</v>
       </c>
       <c r="B8" s="1">
-        <v>0.44511485227000003</v>
+        <v>1.00359036544</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-0</v>
+        <v>3-1</v>
       </c>
       <c r="F8" s="3" t="str">
         <f>VLOOKUP(E8,cs_lookup!$A$2:$B$54,2,FALSE)</f>
@@ -833,23 +833,23 @@
       </c>
       <c r="H8" s="2">
         <f t="shared" si="7"/>
-        <v>0.94</v>
+        <v>2.95</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="8"/>
-        <v>0.45</v>
+        <v>1</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="9"/>
-        <v>1.39</v>
+        <v>3.95</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>0.94088694030799991</v>
+        <v>1.24616643568</v>
       </c>
       <c r="B9" s="1">
-        <v>0.85842388068800002</v>
+        <v>1.0218821889600003</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" si="4"/>
@@ -869,23 +869,23 @@
       </c>
       <c r="H9" s="2">
         <f t="shared" si="7"/>
-        <v>0.94</v>
+        <v>1.25</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="8"/>
-        <v>0.86</v>
+        <v>1.02</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="9"/>
-        <v>1.7999999999999998</v>
+        <v>2.27</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>1.2895605936050001</v>
+        <v>1.2461664356800002</v>
       </c>
       <c r="B10" s="1">
-        <v>1.1537972103680001</v>
+        <v>1.3046454761599999</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" si="4"/>
@@ -905,27 +905,27 @@
       </c>
       <c r="H10" s="2">
         <f t="shared" si="7"/>
-        <v>1.29</v>
+        <v>1.25</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" si="8"/>
-        <v>1.1499999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="9"/>
-        <v>2.44</v>
+        <v>2.5499999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>0.64483029915200007</v>
+        <v>2.3527158986729999</v>
       </c>
       <c r="B11" s="1">
-        <v>1.23396645988</v>
+        <v>0.86726516951200006</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="5"/>
@@ -933,43 +933,43 @@
       </c>
       <c r="E11" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F11" s="3" t="str">
         <f>VLOOKUP(E11,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="7"/>
-        <v>0.64</v>
+        <v>2.35</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" si="8"/>
-        <v>1.23</v>
+        <v>0.87</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="9"/>
-        <v>1.87</v>
+        <v>3.22</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>2.2808166969350001</v>
+        <v>0.64751318310000006</v>
       </c>
       <c r="B12" s="1">
-        <v>1.5383581862880003</v>
+        <v>0.81533938979200005</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>2-2</v>
+        <v>1-1</v>
       </c>
       <c r="F12" s="3" t="str">
         <f>VLOOKUP(E12,cs_lookup!$A$2:$B$54,2,FALSE)</f>
@@ -977,27 +977,27 @@
       </c>
       <c r="H12" s="2">
         <f t="shared" si="7"/>
-        <v>2.2799999999999998</v>
+        <v>0.65</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" si="8"/>
-        <v>1.54</v>
+        <v>0.82</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" si="9"/>
-        <v>3.82</v>
+        <v>1.47</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1.0527494663729999</v>
+        <v>0.43700889732000009</v>
       </c>
       <c r="B13" s="1">
-        <v>0.85471962523200007</v>
+        <v>1.3508993995999998</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="5"/>
@@ -1005,31 +1005,31 @@
       </c>
       <c r="E13" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>0-1</v>
       </c>
       <c r="F13" s="3" t="str">
         <f>VLOOKUP(E13,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="7"/>
-        <v>1.05</v>
+        <v>0.44</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="8"/>
-        <v>0.85</v>
+        <v>1.35</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="9"/>
-        <v>1.9</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1.263259357768</v>
+        <v>0.50991038156400004</v>
       </c>
       <c r="B14" s="1">
-        <v>1.4834168224919999</v>
+        <v>0.83393962935999999</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" si="4"/>
@@ -1049,35 +1049,35 @@
       </c>
       <c r="H14" s="2">
         <f t="shared" si="7"/>
-        <v>1.26</v>
+        <v>0.51</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="8"/>
-        <v>1.48</v>
+        <v>0.83</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="9"/>
-        <v>2.74</v>
+        <v>1.3399999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>0.75188226917099998</v>
+        <v>1.857487817682</v>
       </c>
       <c r="B15" s="1">
-        <v>1.09882727592</v>
+        <v>1.5593970844160001</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-2</v>
       </c>
       <c r="F15" s="3" t="str">
         <f>VLOOKUP(E15,cs_lookup!$A$2:$B$54,2,FALSE)</f>
@@ -1085,59 +1085,59 @@
       </c>
       <c r="H15" s="2">
         <f t="shared" si="7"/>
-        <v>0.75</v>
+        <v>1.86</v>
       </c>
       <c r="I15" s="2">
         <f t="shared" si="8"/>
-        <v>1.1000000000000001</v>
+        <v>1.56</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" si="9"/>
-        <v>1.85</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>2.000193984699</v>
+        <v>1.114390686885</v>
       </c>
       <c r="B16" s="1">
-        <v>0.98894454832799994</v>
+        <v>2.1682279264160003</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="D16" s="4">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
       <c r="E16" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>2-1</v>
+        <v>1-2</v>
       </c>
       <c r="F16" s="3" t="str">
         <f>VLOOKUP(E16,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" si="8"/>
-        <v>0.99</v>
+        <v>2.17</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="9"/>
-        <v>2.99</v>
+        <v>3.2800000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>1.263259357768</v>
+        <v>0.61916260589400007</v>
       </c>
       <c r="B17" s="1">
-        <v>1.611613338016</v>
+        <v>1.5010093315519997</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" si="4"/>
@@ -1157,27 +1157,27 @@
       </c>
       <c r="H17" s="2">
         <f t="shared" si="7"/>
-        <v>1.26</v>
+        <v>0.62</v>
       </c>
       <c r="I17" s="2">
         <f t="shared" si="8"/>
-        <v>1.61</v>
+        <v>1.5</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="9"/>
-        <v>2.87</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>1.9343867264599999</v>
+        <v>1.1572591187019998</v>
       </c>
       <c r="B18" s="1">
-        <v>0.7478796720780001</v>
+        <v>0.81533938979200005</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="5"/>
@@ -1185,31 +1185,31 @@
       </c>
       <c r="E18" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F18" s="3" t="str">
         <f>VLOOKUP(E18,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="7"/>
-        <v>1.93</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="I18" s="2">
         <f t="shared" si="8"/>
-        <v>0.75</v>
+        <v>0.82</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="9"/>
-        <v>2.6799999999999997</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1.3800215866499999</v>
+        <v>0.699270236303</v>
       </c>
       <c r="B19" s="1">
-        <v>0.5087153868280001</v>
+        <v>1.8012591994399996</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="4"/>
@@ -1217,35 +1217,35 @@
       </c>
       <c r="D19" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F19" s="3" t="str">
         <f>VLOOKUP(E19,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="7"/>
-        <v>1.38</v>
+        <v>0.7</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" si="8"/>
-        <v>0.51</v>
+        <v>1.8</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" si="9"/>
-        <v>1.89</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>0.80496166589999996</v>
+        <v>0.76486557234600006</v>
       </c>
       <c r="B20" s="1">
-        <v>0.66763339016000001</v>
+        <v>1.2508161103040001</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="4"/>
@@ -1265,23 +1265,23 @@
       </c>
       <c r="H20" s="2">
         <f t="shared" si="7"/>
-        <v>0.8</v>
+        <v>0.76</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" si="8"/>
-        <v>0.67</v>
+        <v>1.25</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" si="9"/>
-        <v>1.4700000000000002</v>
+        <v>2.0099999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>0.58540545499800001</v>
+        <v>0.66286949519900007</v>
       </c>
       <c r="B21" s="1">
-        <v>1.2399381984000002</v>
+        <v>1.1007961783119999</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="4"/>
@@ -1301,59 +1301,59 @@
       </c>
       <c r="H21" s="2">
         <f t="shared" si="7"/>
-        <v>0.59</v>
+        <v>0.66</v>
       </c>
       <c r="I21" s="2">
         <f t="shared" si="8"/>
-        <v>1.24</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" si="9"/>
-        <v>1.83</v>
+        <v>1.7600000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>1.7642255122099999</v>
+        <v>1.018630883952</v>
       </c>
       <c r="B22" s="1">
-        <v>0.80482238953599983</v>
+        <v>2.4090621811200004</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="D22" s="4">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
       <c r="E22" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>2-1</v>
+        <v>1-2</v>
       </c>
       <c r="F22" s="3" t="str">
         <f>VLOOKUP(E22,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="7"/>
-        <v>1.76</v>
+        <v>1.02</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" si="8"/>
-        <v>0.8</v>
+        <v>2.41</v>
       </c>
       <c r="J22" s="2">
         <f t="shared" si="9"/>
-        <v>2.56</v>
+        <v>3.43</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>0.90567354150000001</v>
+        <v>0.54851663051999999</v>
       </c>
       <c r="B23" s="1">
-        <v>0.39337900282999999</v>
+        <v>0.74352215504000008</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" si="4"/>
@@ -1361,490 +1361,1540 @@
       </c>
       <c r="D23" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-0</v>
+        <v>1-1</v>
       </c>
       <c r="F23" s="3" t="str">
         <f>VLOOKUP(E23,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="H23" s="2">
         <f t="shared" si="7"/>
-        <v>0.91</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I23" s="2">
         <f t="shared" si="8"/>
-        <v>0.39</v>
+        <v>0.74</v>
       </c>
       <c r="J23" s="2">
         <f t="shared" si="9"/>
-        <v>1.3</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="3"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
+      <c r="A24" s="1">
+        <v>1.0578320724960002</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.2427701727999998</v>
+      </c>
+      <c r="C24" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D24" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E24" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F24" s="3" t="str">
+        <f>VLOOKUP(E24,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="7"/>
+        <v>1.06</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="8"/>
+        <v>1.24</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="9"/>
+        <v>2.2999999999999998</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="3"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
+      <c r="A25" s="1">
+        <v>0.70522138166400006</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.8412598092800001</v>
+      </c>
+      <c r="C25" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E25" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F25" s="3" t="str">
+        <f>VLOOKUP(E25,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="7"/>
+        <v>0.71</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="8"/>
+        <v>0.84</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" si="9"/>
+        <v>1.5499999999999998</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="3"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
+      <c r="A26" s="1">
+        <v>2.0372617679039999</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.57358623359999994</v>
+      </c>
+      <c r="C26" s="4">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D26" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E26" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>2-1</v>
+      </c>
+      <c r="F26" s="3" t="str">
+        <f>VLOOKUP(E26,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="7"/>
+        <v>2.04</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="8"/>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="9"/>
+        <v>2.61</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="3"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
+      <c r="A27" s="1">
+        <v>1.4652524266380003</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.57358623359999994</v>
+      </c>
+      <c r="C27" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E27" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F27" s="3" t="str">
+        <f>VLOOKUP(E27,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="7"/>
+        <v>1.47</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="8"/>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="9"/>
+        <v>2.04</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="3"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
+      <c r="A28" s="1">
+        <v>1.4260312400399999</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.9177379737600001</v>
+      </c>
+      <c r="C28" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E28" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F28" s="3" t="str">
+        <f>VLOOKUP(E28,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="7"/>
+        <v>1.43</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="8"/>
+        <v>0.92</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" si="9"/>
+        <v>2.35</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="3"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
+      <c r="A29" s="1">
+        <v>0.76475980549999989</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1.317628204344</v>
+      </c>
+      <c r="C29" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E29" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F29" s="3" t="str">
+        <f>VLOOKUP(E29,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="7"/>
+        <v>0.76</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="8"/>
+        <v>1.32</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="9"/>
+        <v>2.08</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="3"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
+      <c r="A30" s="1">
+        <v>1.1930256009</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.68998792499999995</v>
+      </c>
+      <c r="C30" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E30" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F30" s="3" t="str">
+        <f>VLOOKUP(E30,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="7"/>
+        <v>1.19</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="8"/>
+        <v>0.69</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="9"/>
+        <v>1.88</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="3"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
+      <c r="A31" s="1">
+        <v>3.1797692742999999</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1.4785053762960001</v>
+      </c>
+      <c r="C31" s="4">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E31" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>3-1</v>
+      </c>
+      <c r="F31" s="3" t="str">
+        <f>VLOOKUP(E31,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="7"/>
+        <v>3.18</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="8"/>
+        <v>1.48</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="9"/>
+        <v>4.66</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="3"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
+      <c r="A32" s="1">
+        <v>0.88651801559999999</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.83634899999999979</v>
+      </c>
+      <c r="C32" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E32" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F32" s="3" t="str">
+        <f>VLOOKUP(E32,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="7"/>
+        <v>0.89</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="8"/>
+        <v>0.84</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="9"/>
+        <v>1.73</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="3"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
+      <c r="A33" s="1">
+        <v>0.87603726650000002</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2.156384991456</v>
+      </c>
+      <c r="C33" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="E33" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-2</v>
+      </c>
+      <c r="F33" s="3" t="str">
+        <f>VLOOKUP(E33,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="7"/>
+        <v>0.88</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="8"/>
+        <v>2.16</v>
+      </c>
+      <c r="J33" s="2">
+        <f t="shared" si="9"/>
+        <v>3.04</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="3"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
+      <c r="A34" s="1">
+        <v>1.6894536872999999</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1.3721714395440001</v>
+      </c>
+      <c r="C34" s="4">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E34" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>2-1</v>
+      </c>
+      <c r="F34" s="3" t="str">
+        <f>VLOOKUP(E34,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="7"/>
+        <v>1.69</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="8"/>
+        <v>1.37</v>
+      </c>
+      <c r="J34" s="2">
+        <f t="shared" si="9"/>
+        <v>3.06</v>
+      </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="3"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
+      <c r="A35" s="1">
+        <v>1.8770616733999999</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1.0977626069999999</v>
+      </c>
+      <c r="C35" s="4">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E35" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>2-1</v>
+      </c>
+      <c r="F35" s="3" t="str">
+        <f>VLOOKUP(E35,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="7"/>
+        <v>1.88</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="8"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J35" s="2">
+        <f t="shared" si="9"/>
+        <v>2.98</v>
+      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="3"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
+      <c r="A36" s="1">
+        <v>1.2617703477000002</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.93435410227199989</v>
+      </c>
+      <c r="C36" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E36" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F36" s="3" t="str">
+        <f>VLOOKUP(E36,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="7"/>
+        <v>1.26</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="8"/>
+        <v>0.93</v>
+      </c>
+      <c r="J36" s="2">
+        <f t="shared" si="9"/>
+        <v>2.19</v>
+      </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="3"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
+      <c r="A37" s="1">
+        <v>1.2617703477000002</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.65348856691199997</v>
+      </c>
+      <c r="C37" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D37" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E37" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F37" s="3" t="str">
+        <f>VLOOKUP(E37,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="7"/>
+        <v>1.26</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="8"/>
+        <v>0.65</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="9"/>
+        <v>1.9100000000000001</v>
+      </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="3"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
+      <c r="A38" s="1">
+        <v>0.86339442243599995</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1.4238646721600001</v>
+      </c>
+      <c r="C38" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D38" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E38" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F38" s="3" t="str">
+        <f>VLOOKUP(E38,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="7"/>
+        <v>0.86</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="8"/>
+        <v>1.42</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="9"/>
+        <v>2.2799999999999998</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="3"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
+      <c r="A39" s="1">
+        <v>1.255763316288</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1.08486713104</v>
+      </c>
+      <c r="C39" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E39" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F39" s="3" t="str">
+        <f>VLOOKUP(E39,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="7"/>
+        <v>1.26</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="8"/>
+        <v>1.08</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="9"/>
+        <v>2.34</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="3"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
+      <c r="A40" s="1">
+        <v>1.2169552752500004</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.54843727188799996</v>
+      </c>
+      <c r="C40" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D40" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E40" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F40" s="3" t="str">
+        <f>VLOOKUP(E40,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="7"/>
+        <v>1.22</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="8"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" si="9"/>
+        <v>1.77</v>
+      </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="3"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
+      <c r="A41" s="1">
+        <v>2.0387053240840003</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.65810916996799995</v>
+      </c>
+      <c r="C41" s="4">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D41" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E41" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>2-1</v>
+      </c>
+      <c r="F41" s="3" t="str">
+        <f>VLOOKUP(E41,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="7"/>
+        <v>2.04</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="8"/>
+        <v>0.66</v>
+      </c>
+      <c r="J41" s="2">
+        <f t="shared" si="9"/>
+        <v>2.7</v>
+      </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="3"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
+      <c r="A42" s="1">
+        <v>0.83207065470100017</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.62676958077799994</v>
+      </c>
+      <c r="C42" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D42" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E42" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F42" s="3" t="str">
+        <f>VLOOKUP(E42,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="7"/>
+        <v>0.83</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="8"/>
+        <v>0.63</v>
+      </c>
+      <c r="J42" s="2">
+        <f t="shared" si="9"/>
+        <v>1.46</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="3"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
+      <c r="A43" s="1">
+        <v>1.4728103312400003</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1.55108510944</v>
+      </c>
+      <c r="C43" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D43" s="4">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="E43" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-2</v>
+      </c>
+      <c r="F43" s="3" t="str">
+        <f>VLOOKUP(E43,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" si="7"/>
+        <v>1.47</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="8"/>
+        <v>1.55</v>
+      </c>
+      <c r="J43" s="2">
+        <f t="shared" si="9"/>
+        <v>3.02</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="3"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
+      <c r="A44" s="1">
+        <v>2.4395229600000006</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1.2773877369600002</v>
+      </c>
+      <c r="C44" s="4">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D44" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E44" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>2-1</v>
+      </c>
+      <c r="F44" s="3" t="str">
+        <f>VLOOKUP(E44,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" si="7"/>
+        <v>2.44</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="8"/>
+        <v>1.28</v>
+      </c>
+      <c r="J44" s="2">
+        <f t="shared" si="9"/>
+        <v>3.7199999999999998</v>
+      </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="3"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
+      <c r="A45" s="1">
+        <v>0.34472645485200004</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1.4722046662400001</v>
+      </c>
+      <c r="C45" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D45" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E45" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>0-1</v>
+      </c>
+      <c r="F45" s="3" t="str">
+        <f>VLOOKUP(E45,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H45" s="2">
+        <f t="shared" si="7"/>
+        <v>0.34</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="8"/>
+        <v>1.47</v>
+      </c>
+      <c r="J45" s="2">
+        <f t="shared" si="9"/>
+        <v>1.81</v>
+      </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="3"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
+      <c r="A46" s="1">
+        <v>1.5167865769</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.59898572942400008</v>
+      </c>
+      <c r="C46" s="4">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D46" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E46" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>2-1</v>
+      </c>
+      <c r="F46" s="3" t="str">
+        <f>VLOOKUP(E46,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" si="7"/>
+        <v>1.52</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="8"/>
+        <v>0.6</v>
+      </c>
+      <c r="J46" s="2">
+        <f t="shared" si="9"/>
+        <v>2.12</v>
+      </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="3"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
+      <c r="A47" s="1">
+        <v>1.06001419552</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.69335335560599998</v>
+      </c>
+      <c r="C47" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D47" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E47" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F47" s="3" t="str">
+        <f>VLOOKUP(E47,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" si="7"/>
+        <v>1.06</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="8"/>
+        <v>0.69</v>
+      </c>
+      <c r="J47" s="2">
+        <f t="shared" si="9"/>
+        <v>1.75</v>
+      </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="3"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
+      <c r="A48" s="1">
+        <v>0.82438604002999993</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1.664073052674</v>
+      </c>
+      <c r="C48" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D48" s="4">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="E48" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-2</v>
+      </c>
+      <c r="F48" s="3" t="str">
+        <f>VLOOKUP(E48,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="7"/>
+        <v>0.82</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="8"/>
+        <v>1.66</v>
+      </c>
+      <c r="J48" s="2">
+        <f t="shared" si="9"/>
+        <v>2.48</v>
+      </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="3"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
+      <c r="A49" s="1">
+        <v>0.63598601648000008</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0.83209902438599992</v>
+      </c>
+      <c r="C49" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D49" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E49" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F49" s="3" t="str">
+        <f>VLOOKUP(E49,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="7"/>
+        <v>0.64</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="8"/>
+        <v>0.83</v>
+      </c>
+      <c r="J49" s="2">
+        <f t="shared" si="9"/>
+        <v>1.47</v>
+      </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="3"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
+      <c r="A50" s="1">
+        <v>0.74196493519999984</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1.1233224350750002</v>
+      </c>
+      <c r="C50" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D50" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E50" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F50" s="3" t="str">
+        <f>VLOOKUP(E50,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="7"/>
+        <v>0.74</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="8"/>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="J50" s="2">
+        <f t="shared" si="9"/>
+        <v>1.86</v>
+      </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="3"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
+      <c r="A51" s="1">
+        <v>1.9247439885200004</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1.0461187765439999</v>
+      </c>
+      <c r="C51" s="4">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D51" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E51" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>2-1</v>
+      </c>
+      <c r="F51" s="3" t="str">
+        <f>VLOOKUP(E51,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="7"/>
+        <v>1.92</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="8"/>
+        <v>1.05</v>
+      </c>
+      <c r="J51" s="2">
+        <f t="shared" si="9"/>
+        <v>2.9699999999999998</v>
+      </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="3"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
+      <c r="A52" s="1">
+        <v>1.9432760240040001</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1.664073052674</v>
+      </c>
+      <c r="C52" s="4">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D52" s="4">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="E52" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>2-2</v>
+      </c>
+      <c r="F52" s="3" t="str">
+        <f>VLOOKUP(E52,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="7"/>
+        <v>1.94</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="8"/>
+        <v>1.66</v>
+      </c>
+      <c r="J52" s="2">
+        <f t="shared" si="9"/>
+        <v>3.5999999999999996</v>
+      </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="3"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
+      <c r="A53" s="1">
+        <v>1.236579060045</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1.0400925314579998</v>
+      </c>
+      <c r="C53" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D53" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E53" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F53" s="3" t="str">
+        <f>VLOOKUP(E53,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="7"/>
+        <v>1.24</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="8"/>
+        <v>1.04</v>
+      </c>
+      <c r="J53" s="2">
+        <f t="shared" si="9"/>
+        <v>2.2800000000000002</v>
+      </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="3"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
+      <c r="A54" s="1">
+        <v>1.7767109351900001</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1.4263304742780001</v>
+      </c>
+      <c r="C54" s="4">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D54" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E54" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>2-1</v>
+      </c>
+      <c r="F54" s="3" t="str">
+        <f>VLOOKUP(E54,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="7"/>
+        <v>1.78</v>
+      </c>
+      <c r="I54" s="2">
+        <f t="shared" si="8"/>
+        <v>1.43</v>
+      </c>
+      <c r="J54" s="2">
+        <f t="shared" si="9"/>
+        <v>3.21</v>
+      </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="3"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
+      <c r="A55" s="1">
+        <v>1.9381073865420002</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0.38039384005599997</v>
+      </c>
+      <c r="C55" s="4">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D55" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E55" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>2-0</v>
+      </c>
+      <c r="F55" s="3" t="str">
+        <f>VLOOKUP(E55,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H55" s="2">
+        <f t="shared" si="7"/>
+        <v>1.94</v>
+      </c>
+      <c r="I55" s="2">
+        <f t="shared" si="8"/>
+        <v>0.38</v>
+      </c>
+      <c r="J55" s="2">
+        <f t="shared" si="9"/>
+        <v>2.3199999999999998</v>
+      </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="3"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
+      <c r="A56" s="1">
+        <v>0.89864697351</v>
+      </c>
+      <c r="B56" s="1">
+        <v>1.0999540588050001</v>
+      </c>
+      <c r="C56" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D56" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E56" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F56" s="3" t="str">
+        <f>VLOOKUP(E56,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H56" s="2">
+        <f t="shared" si="7"/>
+        <v>0.9</v>
+      </c>
+      <c r="I56" s="2">
+        <f t="shared" si="8"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J56" s="2">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="3"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
+      <c r="A57" s="1">
+        <v>1.59134151605</v>
+      </c>
+      <c r="B57" s="1">
+        <v>1.8803087423339997</v>
+      </c>
+      <c r="C57" s="4">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D57" s="4">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="E57" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>2-2</v>
+      </c>
+      <c r="F57" s="3" t="str">
+        <f>VLOOKUP(E57,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H57" s="2">
+        <f t="shared" si="7"/>
+        <v>1.59</v>
+      </c>
+      <c r="I57" s="2">
+        <f t="shared" si="8"/>
+        <v>1.88</v>
+      </c>
+      <c r="J57" s="2">
+        <f t="shared" si="9"/>
+        <v>3.4699999999999998</v>
+      </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="3"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
+      <c r="A58" s="1">
+        <v>1.248150425522</v>
+      </c>
+      <c r="B58" s="1">
+        <v>1.5668683971159998</v>
+      </c>
+      <c r="C58" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D58" s="4">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="E58" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-2</v>
+      </c>
+      <c r="F58" s="3" t="str">
+        <f>VLOOKUP(E58,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H58" s="2">
+        <f t="shared" si="7"/>
+        <v>1.25</v>
+      </c>
+      <c r="I58" s="2">
+        <f t="shared" si="8"/>
+        <v>1.57</v>
+      </c>
+      <c r="J58" s="2">
+        <f t="shared" si="9"/>
+        <v>2.8200000000000003</v>
+      </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="3"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
+      <c r="A59" s="1">
+        <v>0.94655286869000022</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0.37605285937900007</v>
+      </c>
+      <c r="C59" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D59" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E59" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-0</v>
+      </c>
+      <c r="F59" s="3" t="str">
+        <f>VLOOKUP(E59,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H59" s="2">
+        <f t="shared" si="7"/>
+        <v>0.95</v>
+      </c>
+      <c r="I59" s="2">
+        <f t="shared" si="8"/>
+        <v>0.38</v>
+      </c>
+      <c r="J59" s="2">
+        <f t="shared" si="9"/>
+        <v>1.33</v>
+      </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="3"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
+      <c r="A60" s="1">
+        <v>0.624002989896</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0.18799309757999999</v>
+      </c>
+      <c r="C60" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D60" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E60" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-0</v>
+      </c>
+      <c r="F60" s="3" t="str">
+        <f>VLOOKUP(E60,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H60" s="2">
+        <f t="shared" si="7"/>
+        <v>0.62</v>
+      </c>
+      <c r="I60" s="2">
+        <f t="shared" si="8"/>
+        <v>0.19</v>
+      </c>
+      <c r="J60" s="2">
+        <f t="shared" si="9"/>
+        <v>0.81</v>
+      </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="3"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
+      <c r="A61" s="1">
+        <v>1.6641413094020001</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0.75215016419699998</v>
+      </c>
+      <c r="C61" s="4">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D61" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E61" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>2-1</v>
+      </c>
+      <c r="F61" s="3" t="str">
+        <f>VLOOKUP(E61,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H61" s="2">
+        <f t="shared" si="7"/>
+        <v>1.66</v>
+      </c>
+      <c r="I61" s="2">
+        <f t="shared" si="8"/>
+        <v>0.75</v>
+      </c>
+      <c r="J61" s="2">
+        <f t="shared" si="9"/>
+        <v>2.41</v>
+      </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="3"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
+      <c r="A62" s="1">
+        <v>0.35101209686399998</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0.37016210139200001</v>
+      </c>
+      <c r="C62" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D62" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E62" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>0-0</v>
+      </c>
+      <c r="F62" s="3" t="str">
+        <f>VLOOKUP(E62,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H62" s="2">
+        <f t="shared" si="7"/>
+        <v>0.35</v>
+      </c>
+      <c r="I62" s="2">
+        <f t="shared" si="8"/>
+        <v>0.37</v>
+      </c>
+      <c r="J62" s="2">
+        <f t="shared" si="9"/>
+        <v>0.72</v>
+      </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="3"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
+      <c r="A63" s="1">
+        <v>1.0909898755199998</v>
+      </c>
+      <c r="B63" s="1">
+        <v>1.0137902675199999</v>
+      </c>
+      <c r="C63" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D63" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E63" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F63" s="3" t="str">
+        <f>VLOOKUP(E63,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H63" s="2">
+        <f t="shared" si="7"/>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="I63" s="2">
+        <f t="shared" si="8"/>
+        <v>1.01</v>
+      </c>
+      <c r="J63" s="2">
+        <f t="shared" si="9"/>
+        <v>2.1</v>
+      </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="3"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
+      <c r="A64" s="1">
+        <v>0.94213761693800002</v>
+      </c>
+      <c r="B64" s="1">
+        <v>0.66566421862499991</v>
+      </c>
+      <c r="C64" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D64" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E64" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F64" s="3" t="str">
+        <f>VLOOKUP(E64,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H64" s="2">
+        <f t="shared" si="7"/>
+        <v>0.94</v>
+      </c>
+      <c r="I64" s="2">
+        <f t="shared" si="8"/>
+        <v>0.67</v>
+      </c>
+      <c r="J64" s="2">
+        <f t="shared" si="9"/>
+        <v>1.6099999999999999</v>
+      </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="3"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
+      <c r="A65" s="1">
+        <v>0.99855589519400001</v>
+      </c>
+      <c r="B65" s="1">
+        <v>0.56410151178800017</v>
+      </c>
+      <c r="C65" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D65" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E65" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F65" s="3" t="str">
+        <f>VLOOKUP(E65,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H65" s="2">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="I65" s="2">
+        <f t="shared" si="8"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="J65" s="2">
+        <f t="shared" si="9"/>
+        <v>1.56</v>
+      </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>

</xml_diff>

<commit_message>
updated odds and fixtures
</commit_message>
<xml_diff>
--- a/CS generator.xlsx
+++ b/CS generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kovan\FDAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6499C124-FE54-4EE6-9E1A-775F951C4D80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE7D96D-FAEC-4A31-9859-E08AD4A1784A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -551,21 +551,21 @@
   <dimension ref="A1:J200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:J65"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
-        <v>2.5230645010799999</v>
+        <v>1.54177941104</v>
       </c>
       <c r="B1" s="2">
-        <v>1.1184931555199999</v>
+        <v>0.60329999519999999</v>
       </c>
       <c r="C1" s="4">
         <f>ROUND(A1,0)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="4">
         <f>ROUND(B1,0)</f>
@@ -573,7 +573,7 @@
       </c>
       <c r="E1" s="5" t="str">
         <f>CONCATENATE(C1,"-",D1)</f>
-        <v>3-1</v>
+        <v>2-1</v>
       </c>
       <c r="F1" s="3" t="str">
         <f>VLOOKUP(E1,cs_lookup!$A$2:$B$54,2,FALSE)</f>
@@ -581,23 +581,23 @@
       </c>
       <c r="H1" s="2">
         <f>ROUND(A1,2)</f>
-        <v>2.52</v>
+        <v>1.54</v>
       </c>
       <c r="I1" s="2">
         <f>ROUND(B1,2)</f>
-        <v>1.1200000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="J1" s="2">
         <f>SUM(H1:I1)</f>
-        <v>3.64</v>
+        <v>2.14</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1.1556708768000001</v>
+        <v>0.93606559832500014</v>
       </c>
       <c r="B2" s="1">
-        <v>0.70253525472000011</v>
+        <v>0.65810916996799995</v>
       </c>
       <c r="C2" s="4">
         <f t="shared" ref="C2" si="0">ROUND(A2,0)</f>
@@ -617,63 +617,63 @@
       </c>
       <c r="H2" s="2">
         <f>ROUND(A2,2)</f>
-        <v>1.1599999999999999</v>
+        <v>0.94</v>
       </c>
       <c r="I2" s="2">
         <f>ROUND(B2,2)</f>
-        <v>0.7</v>
+        <v>0.66</v>
       </c>
       <c r="J2" s="2">
         <f t="shared" ref="J2" si="3">SUM(H2:I2)</f>
-        <v>1.8599999999999999</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2.4395229600000006</v>
+        <v>1.05487682224</v>
       </c>
       <c r="B3" s="1">
-        <v>1.5328932849600001</v>
+        <v>0.82949203680000005</v>
       </c>
       <c r="C3" s="4">
-        <f t="shared" ref="C3:C65" si="4">ROUND(A3,0)</f>
-        <v>2</v>
+        <f t="shared" ref="C3:C66" si="4">ROUND(A3,0)</f>
+        <v>1</v>
       </c>
       <c r="D3" s="4">
-        <f t="shared" ref="D3:D65" si="5">ROUND(B3,0)</f>
-        <v>2</v>
+        <f t="shared" ref="D3:D66" si="5">ROUND(B3,0)</f>
+        <v>1</v>
       </c>
       <c r="E3" s="5" t="str">
-        <f t="shared" ref="E3:E65" si="6">CONCATENATE(C3,"-",D3)</f>
-        <v>2-2</v>
+        <f t="shared" ref="E3:E66" si="6">CONCATENATE(C3,"-",D3)</f>
+        <v>1-1</v>
       </c>
       <c r="F3" s="3" t="str">
         <f>VLOOKUP(E3,cs_lookup!$A$2:$B$54,2,FALSE)</f>
         <v>X</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H65" si="7">ROUND(A3,2)</f>
-        <v>2.44</v>
+        <f t="shared" ref="H3:H66" si="7">ROUND(A3,2)</f>
+        <v>1.05</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I65" si="8">ROUND(B3,2)</f>
-        <v>1.53</v>
+        <f t="shared" ref="I3:I66" si="8">ROUND(B3,2)</f>
+        <v>0.83</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J65" si="9">SUM(H3:I3)</f>
-        <v>3.9699999999999998</v>
+        <f t="shared" ref="J3:J66" si="9">SUM(H3:I3)</f>
+        <v>1.88</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1.3594133854800001</v>
+        <v>2.29701967488</v>
       </c>
       <c r="B4" s="1">
-        <v>1.10390540416</v>
+        <v>1.3573340760000001</v>
       </c>
       <c r="C4" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" si="5"/>
@@ -681,31 +681,31 @@
       </c>
       <c r="E4" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F4" s="3" t="str">
         <f>VLOOKUP(E4,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="7"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" si="8"/>
         <v>1.36</v>
       </c>
-      <c r="I4" s="2">
-        <f t="shared" si="8"/>
-        <v>1.1000000000000001</v>
-      </c>
       <c r="J4" s="2">
         <f t="shared" si="9"/>
-        <v>2.46</v>
+        <v>3.66</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>0.90631558836000004</v>
+        <v>0.95512221360000005</v>
       </c>
       <c r="B5" s="1">
-        <v>1.4598859849600001</v>
+        <v>0.9049499928000001</v>
       </c>
       <c r="C5" s="4">
         <f t="shared" si="4"/>
@@ -725,23 +725,23 @@
       </c>
       <c r="H5" s="2">
         <f t="shared" si="7"/>
-        <v>0.91</v>
+        <v>0.96</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="8"/>
-        <v>1.46</v>
+        <v>0.9</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="9"/>
-        <v>2.37</v>
+        <v>1.8599999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>0.83081428975999994</v>
+        <v>1.1443227139200001</v>
       </c>
       <c r="B6" s="1">
-        <v>0.82119211648000012</v>
+        <v>0.66362999472000006</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="4"/>
@@ -761,27 +761,27 @@
       </c>
       <c r="H6" s="2">
         <f t="shared" si="7"/>
-        <v>0.83</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" si="8"/>
-        <v>0.82</v>
+        <v>0.66</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="9"/>
-        <v>1.65</v>
+        <v>1.7999999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>1.5710930225999999</v>
+        <v>0.74897321575999998</v>
       </c>
       <c r="B7" s="1">
-        <v>0.83028802872000007</v>
+        <v>0.82949203680000005</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="5"/>
@@ -789,15 +789,15 @@
       </c>
       <c r="E7" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F7" s="3" t="str">
         <f>VLOOKUP(E7,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="7"/>
-        <v>1.57</v>
+        <v>0.75</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="8"/>
@@ -805,51 +805,51 @@
       </c>
       <c r="J7" s="2">
         <f t="shared" si="9"/>
-        <v>2.4</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>2.9538841436799999</v>
+        <v>0.89261535272000003</v>
       </c>
       <c r="B8" s="1">
-        <v>1.00359036544</v>
+        <v>2.4128727042399998</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>3-1</v>
+        <v>1-2</v>
       </c>
       <c r="F8" s="3" t="str">
         <f>VLOOKUP(E8,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="7"/>
-        <v>2.95</v>
+        <v>0.89</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>2.41</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="9"/>
-        <v>3.95</v>
+        <v>3.3000000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>1.24616643568</v>
+        <v>0.61168903272000008</v>
       </c>
       <c r="B9" s="1">
-        <v>1.0218821889600003</v>
+        <v>0.91239124096000002</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" si="4"/>
@@ -869,23 +869,23 @@
       </c>
       <c r="H9" s="2">
         <f t="shared" si="7"/>
-        <v>1.25</v>
+        <v>0.61</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="8"/>
-        <v>1.02</v>
+        <v>0.91</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="9"/>
-        <v>2.27</v>
+        <v>1.52</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>1.2461664356800002</v>
+        <v>1.2235053415600001</v>
       </c>
       <c r="B10" s="1">
-        <v>1.3046454761599999</v>
+        <v>0.84454726272000002</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" si="4"/>
@@ -905,23 +905,23 @@
       </c>
       <c r="H10" s="2">
         <f t="shared" si="7"/>
-        <v>1.25</v>
+        <v>1.22</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" si="8"/>
-        <v>1.3</v>
+        <v>0.84</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="9"/>
-        <v>2.5499999999999998</v>
+        <v>2.06</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>2.3527158986729999</v>
+        <v>1.6852579148400002</v>
       </c>
       <c r="B11" s="1">
-        <v>0.86726516951200006</v>
+        <v>0.63341044704000005</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" si="4"/>
@@ -941,27 +941,27 @@
       </c>
       <c r="H11" s="2">
         <f t="shared" si="7"/>
-        <v>2.35</v>
+        <v>1.69</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" si="8"/>
-        <v>0.87</v>
+        <v>0.63</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="9"/>
-        <v>3.22</v>
+        <v>2.3199999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>0.64751318310000006</v>
+        <v>2.4198503791770003</v>
       </c>
       <c r="B12" s="1">
-        <v>0.81533938979200005</v>
+        <v>1.334217184496</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="5"/>
@@ -969,35 +969,35 @@
       </c>
       <c r="E12" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F12" s="3" t="str">
         <f>VLOOKUP(E12,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" si="7"/>
-        <v>0.65</v>
+        <v>2.42</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" si="8"/>
-        <v>0.82</v>
+        <v>1.33</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" si="9"/>
-        <v>1.47</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>0.43700889732000009</v>
+        <v>1.5295811416380001</v>
       </c>
       <c r="B13" s="1">
-        <v>1.3508993995999998</v>
+        <v>1.0006228890559998</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="5"/>
@@ -1005,43 +1005,43 @@
       </c>
       <c r="E13" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>0-1</v>
+        <v>2-1</v>
       </c>
       <c r="F13" s="3" t="str">
         <f>VLOOKUP(E13,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="7"/>
-        <v>0.44</v>
+        <v>1.53</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="8"/>
-        <v>1.35</v>
+        <v>1</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="9"/>
-        <v>1.79</v>
+        <v>2.5300000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>0.50991038156400004</v>
+        <v>2.4766504235760003</v>
       </c>
       <c r="B14" s="1">
-        <v>0.83393962935999999</v>
+        <v>1.7345303390240001</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-2</v>
       </c>
       <c r="F14" s="3" t="str">
         <f>VLOOKUP(E14,cs_lookup!$A$2:$B$54,2,FALSE)</f>
@@ -1049,35 +1049,35 @@
       </c>
       <c r="H14" s="2">
         <f t="shared" si="7"/>
-        <v>0.51</v>
+        <v>2.48</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="8"/>
-        <v>0.83</v>
+        <v>1.73</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="9"/>
-        <v>1.3399999999999999</v>
+        <v>4.21</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>1.857487817682</v>
+        <v>1.2018244686480002</v>
       </c>
       <c r="B15" s="1">
-        <v>1.5593970844160001</v>
+        <v>1.000712889016</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="4">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>2-2</v>
+        <v>1-1</v>
       </c>
       <c r="F15" s="3" t="str">
         <f>VLOOKUP(E15,cs_lookup!$A$2:$B$54,2,FALSE)</f>
@@ -1085,59 +1085,59 @@
       </c>
       <c r="H15" s="2">
         <f t="shared" si="7"/>
-        <v>1.86</v>
+        <v>1.2</v>
       </c>
       <c r="I15" s="2">
         <f t="shared" si="8"/>
-        <v>1.56</v>
+        <v>1</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" si="9"/>
-        <v>3.42</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>1.114390686885</v>
+        <v>2.3792862227200002</v>
       </c>
       <c r="B16" s="1">
-        <v>2.1682279264160003</v>
+        <v>1.0191742372400001</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="4">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-2</v>
+        <v>2-1</v>
       </c>
       <c r="F16" s="3" t="str">
         <f>VLOOKUP(E16,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="7"/>
-        <v>1.1100000000000001</v>
+        <v>2.38</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" si="8"/>
-        <v>2.17</v>
+        <v>1.02</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="9"/>
-        <v>3.2800000000000002</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>0.61916260589400007</v>
+        <v>1.2454213612049998</v>
       </c>
       <c r="B17" s="1">
-        <v>1.5010093315519997</v>
+        <v>0.66710859224800012</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" si="4"/>
@@ -1145,107 +1145,107 @@
       </c>
       <c r="D17" s="4">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-2</v>
+        <v>1-1</v>
       </c>
       <c r="F17" s="3" t="str">
         <f>VLOOKUP(E17,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>X</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="7"/>
-        <v>0.62</v>
+        <v>1.25</v>
       </c>
       <c r="I17" s="2">
         <f t="shared" si="8"/>
-        <v>1.5</v>
+        <v>0.67</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="9"/>
-        <v>2.12</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>1.1572591187019998</v>
+        <v>1.6024326248640002</v>
       </c>
       <c r="B18" s="1">
-        <v>0.81533938979200005</v>
+        <v>0.45026979987999999</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-0</v>
       </c>
       <c r="F18" s="3" t="str">
         <f>VLOOKUP(E18,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="7"/>
-        <v>1.1599999999999999</v>
+        <v>1.6</v>
       </c>
       <c r="I18" s="2">
         <f t="shared" si="8"/>
-        <v>0.82</v>
+        <v>0.45</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="9"/>
-        <v>1.98</v>
+        <v>2.0500000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>0.699270236303</v>
+        <v>2.214209083674</v>
       </c>
       <c r="B19" s="1">
-        <v>1.8012591994399996</v>
+        <v>0.52532976651999996</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-2</v>
+        <v>2-1</v>
       </c>
       <c r="F19" s="3" t="str">
         <f>VLOOKUP(E19,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="7"/>
-        <v>0.7</v>
+        <v>2.21</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" si="8"/>
-        <v>1.8</v>
+        <v>0.53</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" si="9"/>
-        <v>2.5</v>
+        <v>2.74</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>0.76486557234600006</v>
+        <v>1.223692912233</v>
       </c>
       <c r="B20" s="1">
-        <v>1.2508161103040001</v>
+        <v>0.64208526959200007</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="4"/>
@@ -1265,23 +1265,23 @@
       </c>
       <c r="H20" s="2">
         <f t="shared" si="7"/>
-        <v>0.76</v>
+        <v>1.22</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" si="8"/>
-        <v>1.25</v>
+        <v>0.64</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" si="9"/>
-        <v>2.0099999999999998</v>
+        <v>1.8599999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>0.66286949519900007</v>
+        <v>1.38470227214</v>
       </c>
       <c r="B21" s="1">
-        <v>1.1007961783119999</v>
+        <v>0.82351678256000005</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="4"/>
@@ -1301,59 +1301,59 @@
       </c>
       <c r="H21" s="2">
         <f t="shared" si="7"/>
-        <v>0.66</v>
+        <v>1.38</v>
       </c>
       <c r="I21" s="2">
         <f t="shared" si="8"/>
-        <v>1.1000000000000001</v>
+        <v>0.82</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" si="9"/>
-        <v>1.7600000000000002</v>
+        <v>2.1999999999999997</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>1.018630883952</v>
+        <v>1.8427755192440003</v>
       </c>
       <c r="B22" s="1">
-        <v>2.4090621811200004</v>
+        <v>1.192538360056</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-2</v>
+        <v>2-1</v>
       </c>
       <c r="F22" s="3" t="str">
         <f>VLOOKUP(E22,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="7"/>
-        <v>1.02</v>
+        <v>1.84</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" si="8"/>
-        <v>2.41</v>
+        <v>1.19</v>
       </c>
       <c r="J22" s="2">
         <f t="shared" si="9"/>
-        <v>3.43</v>
+        <v>3.0300000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>0.54851663051999999</v>
+        <v>1.398540472606</v>
       </c>
       <c r="B23" s="1">
-        <v>0.74352215504000008</v>
+        <v>2.0181079931360002</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" si="4"/>
@@ -1361,35 +1361,35 @@
       </c>
       <c r="D23" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F23" s="3" t="str">
         <f>VLOOKUP(E23,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="H23" s="2">
         <f t="shared" si="7"/>
-        <v>0.55000000000000004</v>
+        <v>1.4</v>
       </c>
       <c r="I23" s="2">
         <f t="shared" si="8"/>
-        <v>0.74</v>
+        <v>2.02</v>
       </c>
       <c r="J23" s="2">
         <f t="shared" si="9"/>
-        <v>1.29</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>1.0578320724960002</v>
+        <v>1.1204159761079999</v>
       </c>
       <c r="B24" s="1">
-        <v>1.2427701727999998</v>
+        <v>1.0515747616000002</v>
       </c>
       <c r="C24" s="4">
         <f t="shared" si="4"/>
@@ -1409,27 +1409,27 @@
       </c>
       <c r="H24" s="2">
         <f t="shared" si="7"/>
-        <v>1.06</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I24" s="2">
         <f t="shared" si="8"/>
-        <v>1.24</v>
+        <v>1.05</v>
       </c>
       <c r="J24" s="2">
         <f t="shared" si="9"/>
-        <v>2.2999999999999998</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>0.70522138166400006</v>
+        <v>1.8334315961280001</v>
       </c>
       <c r="B25" s="1">
-        <v>0.8412598092800001</v>
+        <v>0.84125980928000021</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="5"/>
@@ -1437,15 +1437,15 @@
       </c>
       <c r="E25" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F25" s="3" t="str">
         <f>VLOOKUP(E25,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" si="7"/>
-        <v>0.71</v>
+        <v>1.83</v>
       </c>
       <c r="I25" s="2">
         <f t="shared" si="8"/>
@@ -1453,19 +1453,19 @@
       </c>
       <c r="J25" s="2">
         <f t="shared" si="9"/>
-        <v>1.5499999999999998</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>2.0372617679039999</v>
+        <v>1.3164119134200001</v>
       </c>
       <c r="B26" s="1">
-        <v>0.57358623359999994</v>
+        <v>0.51622761024000008</v>
       </c>
       <c r="C26" s="4">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" s="4">
         <f t="shared" si="5"/>
@@ -1473,31 +1473,31 @@
       </c>
       <c r="E26" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F26" s="3" t="str">
         <f>VLOOKUP(E26,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" si="7"/>
-        <v>2.04</v>
+        <v>1.32</v>
       </c>
       <c r="I26" s="2">
         <f t="shared" si="8"/>
-        <v>0.56999999999999995</v>
+        <v>0.52</v>
       </c>
       <c r="J26" s="2">
         <f t="shared" si="9"/>
-        <v>2.61</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>1.4652524266380003</v>
+        <v>0.65820595671000004</v>
       </c>
       <c r="B27" s="1">
-        <v>0.57358623359999994</v>
+        <v>1.3670471900800001</v>
       </c>
       <c r="C27" s="4">
         <f t="shared" si="4"/>
@@ -1517,27 +1517,27 @@
       </c>
       <c r="H27" s="2">
         <f t="shared" si="7"/>
-        <v>1.47</v>
+        <v>0.66</v>
       </c>
       <c r="I27" s="2">
         <f t="shared" si="8"/>
-        <v>0.56999999999999995</v>
+        <v>1.37</v>
       </c>
       <c r="J27" s="2">
         <f t="shared" si="9"/>
-        <v>2.04</v>
+        <v>2.0300000000000002</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>1.4260312400399999</v>
+        <v>1.6297314180839999</v>
       </c>
       <c r="B28" s="1">
-        <v>0.9177379737600001</v>
+        <v>1.2618897139200003</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" si="5"/>
@@ -1545,31 +1545,31 @@
       </c>
       <c r="E28" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F28" s="3" t="str">
         <f>VLOOKUP(E28,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" si="7"/>
-        <v>1.43</v>
+        <v>1.63</v>
       </c>
       <c r="I28" s="2">
         <f t="shared" si="8"/>
-        <v>0.92</v>
+        <v>1.26</v>
       </c>
       <c r="J28" s="2">
         <f t="shared" si="9"/>
-        <v>2.35</v>
+        <v>2.8899999999999997</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>0.76475980549999989</v>
+        <v>0.54851663051999999</v>
       </c>
       <c r="B29" s="1">
-        <v>1.317628204344</v>
+        <v>1.6825196185600004</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" si="4"/>
@@ -1577,75 +1577,75 @@
       </c>
       <c r="D29" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F29" s="3" t="str">
         <f>VLOOKUP(E29,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="H29" s="2">
         <f t="shared" si="7"/>
-        <v>0.76</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I29" s="2">
         <f t="shared" si="8"/>
-        <v>1.32</v>
+        <v>1.68</v>
       </c>
       <c r="J29" s="2">
         <f t="shared" si="9"/>
-        <v>2.08</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>1.1930256009</v>
+        <v>2.1313226212740002</v>
       </c>
       <c r="B30" s="1">
-        <v>0.68998792499999995</v>
+        <v>0.26767357568</v>
       </c>
       <c r="C30" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D30" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-0</v>
       </c>
       <c r="F30" s="3" t="str">
         <f>VLOOKUP(E30,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="7"/>
-        <v>1.19</v>
+        <v>2.13</v>
       </c>
       <c r="I30" s="2">
         <f t="shared" si="8"/>
-        <v>0.69</v>
+        <v>0.27</v>
       </c>
       <c r="J30" s="2">
         <f t="shared" si="9"/>
-        <v>1.88</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>3.1797692742999999</v>
+        <v>1.1988583493040001</v>
       </c>
       <c r="B31" s="1">
-        <v>1.4785053762960001</v>
+        <v>1.4722046662400003</v>
       </c>
       <c r="C31" s="4">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D31" s="4">
         <f t="shared" si="5"/>
@@ -1653,43 +1653,43 @@
       </c>
       <c r="E31" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>3-1</v>
+        <v>1-1</v>
       </c>
       <c r="F31" s="3" t="str">
         <f>VLOOKUP(E31,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" si="7"/>
-        <v>3.18</v>
+        <v>1.2</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" si="8"/>
-        <v>1.48</v>
+        <v>1.47</v>
       </c>
       <c r="J31" s="2">
         <f t="shared" si="9"/>
-        <v>4.66</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>0.88651801559999999</v>
+        <v>1.504453615182</v>
       </c>
       <c r="B32" s="1">
-        <v>0.83634899999999979</v>
+        <v>1.6251609952000001</v>
       </c>
       <c r="C32" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E32" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-2</v>
       </c>
       <c r="F32" s="3" t="str">
         <f>VLOOKUP(E32,cs_lookup!$A$2:$B$54,2,FALSE)</f>
@@ -1697,23 +1697,23 @@
       </c>
       <c r="H32" s="2">
         <f t="shared" si="7"/>
-        <v>0.89</v>
+        <v>1.5</v>
       </c>
       <c r="I32" s="2">
         <f t="shared" si="8"/>
-        <v>0.84</v>
+        <v>1.63</v>
       </c>
       <c r="J32" s="2">
         <f t="shared" si="9"/>
-        <v>1.73</v>
+        <v>3.13</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>0.87603726650000002</v>
+        <v>1.3241161541519999</v>
       </c>
       <c r="B33" s="1">
-        <v>2.156384991456</v>
+        <v>0.1911954112</v>
       </c>
       <c r="C33" s="4">
         <f t="shared" si="4"/>
@@ -1721,35 +1721,35 @@
       </c>
       <c r="D33" s="4">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E33" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-2</v>
+        <v>1-0</v>
       </c>
       <c r="F33" s="3" t="str">
         <f>VLOOKUP(E33,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H33" s="2">
         <f t="shared" si="7"/>
-        <v>0.88</v>
+        <v>1.32</v>
       </c>
       <c r="I33" s="2">
         <f t="shared" si="8"/>
-        <v>2.16</v>
+        <v>0.19</v>
       </c>
       <c r="J33" s="2">
         <f t="shared" si="9"/>
-        <v>3.04</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>1.6894536872999999</v>
+        <v>1.5985344666060002</v>
       </c>
       <c r="B34" s="1">
-        <v>1.3721714395440001</v>
+        <v>0.68830348032000011</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="4"/>
@@ -1769,23 +1769,23 @@
       </c>
       <c r="H34" s="2">
         <f t="shared" si="7"/>
-        <v>1.69</v>
+        <v>1.6</v>
       </c>
       <c r="I34" s="2">
         <f t="shared" si="8"/>
-        <v>1.37</v>
+        <v>0.69</v>
       </c>
       <c r="J34" s="2">
         <f t="shared" si="9"/>
-        <v>3.06</v>
+        <v>2.29</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>1.8770616733999999</v>
+        <v>1.7761871856960001</v>
       </c>
       <c r="B35" s="1">
-        <v>1.0977626069999999</v>
+        <v>0.42486980288000004</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="4"/>
@@ -1793,11 +1793,11 @@
       </c>
       <c r="D35" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>2-1</v>
+        <v>2-0</v>
       </c>
       <c r="F35" s="3" t="str">
         <f>VLOOKUP(E35,cs_lookup!$A$2:$B$54,2,FALSE)</f>
@@ -1805,27 +1805,27 @@
       </c>
       <c r="H35" s="2">
         <f t="shared" si="7"/>
-        <v>1.88</v>
+        <v>1.78</v>
       </c>
       <c r="I35" s="2">
         <f t="shared" si="8"/>
-        <v>1.1000000000000001</v>
+        <v>0.42</v>
       </c>
       <c r="J35" s="2">
         <f t="shared" si="9"/>
-        <v>2.98</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>1.2617703477000002</v>
+        <v>2.3995778521859998</v>
       </c>
       <c r="B36" s="1">
-        <v>0.93435410227199989</v>
+        <v>1.1591540188830001</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D36" s="4">
         <f t="shared" si="5"/>
@@ -1833,35 +1833,35 @@
       </c>
       <c r="E36" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F36" s="3" t="str">
         <f>VLOOKUP(E36,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="H36" s="2">
         <f t="shared" si="7"/>
-        <v>1.26</v>
+        <v>2.4</v>
       </c>
       <c r="I36" s="2">
         <f t="shared" si="8"/>
-        <v>0.93</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="J36" s="2">
         <f t="shared" si="9"/>
-        <v>2.19</v>
+        <v>3.5599999999999996</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>1.2617703477000002</v>
+        <v>1.7900779020350002</v>
       </c>
       <c r="B37" s="1">
-        <v>0.65348856691199997</v>
+        <v>1.0461187765439999</v>
       </c>
       <c r="C37" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D37" s="4">
         <f t="shared" si="5"/>
@@ -1869,43 +1869,43 @@
       </c>
       <c r="E37" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F37" s="3" t="str">
         <f>VLOOKUP(E37,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="H37" s="2">
         <f t="shared" si="7"/>
-        <v>1.26</v>
+        <v>1.79</v>
       </c>
       <c r="I37" s="2">
         <f t="shared" si="8"/>
-        <v>0.65</v>
+        <v>1.05</v>
       </c>
       <c r="J37" s="2">
         <f t="shared" si="9"/>
-        <v>1.9100000000000001</v>
+        <v>2.84</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>0.86339442243599995</v>
+        <v>1.885737714</v>
       </c>
       <c r="B38" s="1">
-        <v>1.4238646721600001</v>
+        <v>2.4688816878160003</v>
       </c>
       <c r="C38" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D38" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E38" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-2</v>
       </c>
       <c r="F38" s="3" t="str">
         <f>VLOOKUP(E38,cs_lookup!$A$2:$B$54,2,FALSE)</f>
@@ -1913,59 +1913,59 @@
       </c>
       <c r="H38" s="2">
         <f t="shared" si="7"/>
-        <v>0.86</v>
+        <v>1.89</v>
       </c>
       <c r="I38" s="2">
         <f t="shared" si="8"/>
-        <v>1.42</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="J38" s="2">
         <f t="shared" si="9"/>
-        <v>2.2799999999999998</v>
+        <v>4.3600000000000003</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>1.255763316288</v>
+        <v>2.399997999</v>
       </c>
       <c r="B39" s="1">
-        <v>1.08486713104</v>
+        <v>0.22049708866500001</v>
       </c>
       <c r="C39" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D39" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-0</v>
       </c>
       <c r="F39" s="3" t="str">
         <f>VLOOKUP(E39,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" si="7"/>
-        <v>1.26</v>
+        <v>2.4</v>
       </c>
       <c r="I39" s="2">
         <f t="shared" si="8"/>
-        <v>1.08</v>
+        <v>0.22</v>
       </c>
       <c r="J39" s="2">
         <f t="shared" si="9"/>
-        <v>2.34</v>
+        <v>2.62</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>1.2169552752500004</v>
+        <v>1.1250224999999998</v>
       </c>
       <c r="B40" s="1">
-        <v>0.54843727188799996</v>
+        <v>0.72011965872999995</v>
       </c>
       <c r="C40" s="4">
         <f t="shared" si="4"/>
@@ -1985,27 +1985,27 @@
       </c>
       <c r="H40" s="2">
         <f t="shared" si="7"/>
-        <v>1.22</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="I40" s="2">
         <f t="shared" si="8"/>
-        <v>0.55000000000000004</v>
+        <v>0.72</v>
       </c>
       <c r="J40" s="2">
         <f t="shared" si="9"/>
-        <v>1.77</v>
+        <v>1.8499999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>2.0387053240840003</v>
+        <v>1.214390954</v>
       </c>
       <c r="B41" s="1">
-        <v>0.65810916996799995</v>
+        <v>1.2933353070899998</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D41" s="4">
         <f t="shared" si="5"/>
@@ -2013,31 +2013,31 @@
       </c>
       <c r="E41" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F41" s="3" t="str">
         <f>VLOOKUP(E41,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="H41" s="2">
         <f t="shared" si="7"/>
-        <v>2.04</v>
+        <v>1.21</v>
       </c>
       <c r="I41" s="2">
         <f t="shared" si="8"/>
-        <v>0.66</v>
+        <v>1.29</v>
       </c>
       <c r="J41" s="2">
         <f t="shared" si="9"/>
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>0.83207065470100017</v>
+        <v>1.1250224999999998</v>
       </c>
       <c r="B42" s="1">
-        <v>0.62676958077799994</v>
+        <v>2.2632617853599997</v>
       </c>
       <c r="C42" s="4">
         <f t="shared" si="4"/>
@@ -2045,111 +2045,111 @@
       </c>
       <c r="D42" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F42" s="3" t="str">
         <f>VLOOKUP(E42,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="H42" s="2">
         <f t="shared" si="7"/>
-        <v>0.83</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="I42" s="2">
         <f t="shared" si="8"/>
-        <v>0.63</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="J42" s="2">
         <f t="shared" si="9"/>
-        <v>1.46</v>
+        <v>3.3899999999999997</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>1.4728103312400003</v>
+        <v>2.8636217060880003</v>
       </c>
       <c r="B43" s="1">
-        <v>1.55108510944</v>
+        <v>1.2642842713499998</v>
       </c>
       <c r="C43" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D43" s="4">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E43" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-2</v>
+        <v>3-1</v>
       </c>
       <c r="F43" s="3" t="str">
         <f>VLOOKUP(E43,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H43" s="2">
         <f t="shared" si="7"/>
-        <v>1.47</v>
+        <v>2.86</v>
       </c>
       <c r="I43" s="2">
         <f t="shared" si="8"/>
-        <v>1.55</v>
+        <v>1.26</v>
       </c>
       <c r="J43" s="2">
         <f t="shared" si="9"/>
-        <v>3.02</v>
+        <v>4.12</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>2.4395229600000006</v>
+        <v>1.017335836088</v>
       </c>
       <c r="B44" s="1">
-        <v>1.2773877369600002</v>
+        <v>1.8390509862750002</v>
       </c>
       <c r="C44" s="4">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D44" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E44" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>2-1</v>
+        <v>1-2</v>
       </c>
       <c r="F44" s="3" t="str">
         <f>VLOOKUP(E44,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H44" s="2">
         <f t="shared" si="7"/>
-        <v>2.44</v>
+        <v>1.02</v>
       </c>
       <c r="I44" s="2">
         <f t="shared" si="8"/>
-        <v>1.28</v>
+        <v>1.84</v>
       </c>
       <c r="J44" s="2">
         <f t="shared" si="9"/>
-        <v>3.7199999999999998</v>
+        <v>2.8600000000000003</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>0.34472645485200004</v>
+        <v>1.9780634302000002</v>
       </c>
       <c r="B45" s="1">
-        <v>1.4722046662400001</v>
+        <v>0.89388572314000003</v>
       </c>
       <c r="C45" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D45" s="4">
         <f t="shared" si="5"/>
@@ -2157,31 +2157,31 @@
       </c>
       <c r="E45" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>0-1</v>
+        <v>2-1</v>
       </c>
       <c r="F45" s="3" t="str">
         <f>VLOOKUP(E45,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H45" s="2">
         <f t="shared" si="7"/>
-        <v>0.34</v>
+        <v>1.98</v>
       </c>
       <c r="I45" s="2">
         <f t="shared" si="8"/>
-        <v>1.47</v>
+        <v>0.89</v>
       </c>
       <c r="J45" s="2">
         <f t="shared" si="9"/>
-        <v>1.81</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>1.5167865769</v>
+        <v>2.3266184152640004</v>
       </c>
       <c r="B46" s="1">
-        <v>0.59898572942400008</v>
+        <v>2.8223915293599999</v>
       </c>
       <c r="C46" s="4">
         <f t="shared" si="4"/>
@@ -2189,39 +2189,39 @@
       </c>
       <c r="D46" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E46" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>2-1</v>
+        <v>2-3</v>
       </c>
       <c r="F46" s="3" t="str">
         <f>VLOOKUP(E46,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H46" s="2">
         <f t="shared" si="7"/>
-        <v>1.52</v>
+        <v>2.33</v>
       </c>
       <c r="I46" s="2">
         <f t="shared" si="8"/>
-        <v>0.6</v>
+        <v>2.82</v>
       </c>
       <c r="J46" s="2">
         <f t="shared" si="9"/>
-        <v>2.12</v>
+        <v>5.15</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>1.06001419552</v>
+        <v>1.9592148507360003</v>
       </c>
       <c r="B47" s="1">
-        <v>0.69335335560599998</v>
+        <v>0.91950674300000002</v>
       </c>
       <c r="C47" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D47" s="4">
         <f t="shared" si="5"/>
@@ -2229,35 +2229,35 @@
       </c>
       <c r="E47" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F47" s="3" t="str">
         <f>VLOOKUP(E47,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="H47" s="2">
         <f t="shared" si="7"/>
-        <v>1.06</v>
+        <v>1.96</v>
       </c>
       <c r="I47" s="2">
         <f t="shared" si="8"/>
-        <v>0.69</v>
+        <v>0.92</v>
       </c>
       <c r="J47" s="2">
         <f t="shared" si="9"/>
-        <v>1.75</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>0.82438604002999993</v>
+        <v>0.38225713125600003</v>
       </c>
       <c r="B48" s="1">
-        <v>1.664073052674</v>
+        <v>1.5416337810960004</v>
       </c>
       <c r="C48" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" s="4">
         <f t="shared" si="5"/>
@@ -2265,7 +2265,7 @@
       </c>
       <c r="E48" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-2</v>
+        <v>0-2</v>
       </c>
       <c r="F48" s="3" t="str">
         <f>VLOOKUP(E48,cs_lookup!$A$2:$B$54,2,FALSE)</f>
@@ -2273,35 +2273,35 @@
       </c>
       <c r="H48" s="2">
         <f t="shared" si="7"/>
-        <v>0.82</v>
+        <v>0.38</v>
       </c>
       <c r="I48" s="2">
         <f t="shared" si="8"/>
-        <v>1.66</v>
+        <v>1.54</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" si="9"/>
-        <v>2.48</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>0.63598601648000008</v>
+        <v>2.4078974195880001</v>
       </c>
       <c r="B49" s="1">
-        <v>0.83209902438599992</v>
+        <v>1.9566923932800004</v>
       </c>
       <c r="C49" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D49" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E49" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-2</v>
       </c>
       <c r="F49" s="3" t="str">
         <f>VLOOKUP(E49,cs_lookup!$A$2:$B$54,2,FALSE)</f>
@@ -2309,27 +2309,27 @@
       </c>
       <c r="H49" s="2">
         <f t="shared" si="7"/>
-        <v>0.64</v>
+        <v>2.41</v>
       </c>
       <c r="I49" s="2">
         <f t="shared" si="8"/>
-        <v>0.83</v>
+        <v>1.96</v>
       </c>
       <c r="J49" s="2">
         <f t="shared" si="9"/>
-        <v>1.47</v>
+        <v>4.37</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>0.74196493519999984</v>
+        <v>1.6147601250570001</v>
       </c>
       <c r="B50" s="1">
-        <v>1.1233224350750002</v>
+        <v>1.3874216531040002</v>
       </c>
       <c r="C50" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50" s="4">
         <f t="shared" si="5"/>
@@ -2337,67 +2337,67 @@
       </c>
       <c r="E50" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F50" s="3" t="str">
         <f>VLOOKUP(E50,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="H50" s="2">
         <f t="shared" si="7"/>
-        <v>0.74</v>
+        <v>1.61</v>
       </c>
       <c r="I50" s="2">
         <f t="shared" si="8"/>
-        <v>1.1200000000000001</v>
+        <v>1.39</v>
       </c>
       <c r="J50" s="2">
         <f t="shared" si="9"/>
-        <v>1.86</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>1.9247439885200004</v>
+        <v>0.6880528347660001</v>
       </c>
       <c r="B51" s="1">
-        <v>1.0461187765439999</v>
+        <v>1.9211059409760003</v>
       </c>
       <c r="C51" s="4">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E51" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>2-1</v>
+        <v>1-2</v>
       </c>
       <c r="F51" s="3" t="str">
         <f>VLOOKUP(E51,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H51" s="2">
         <f t="shared" si="7"/>
+        <v>0.69</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="8"/>
         <v>1.92</v>
       </c>
-      <c r="I51" s="2">
-        <f t="shared" si="8"/>
-        <v>1.05</v>
-      </c>
       <c r="J51" s="2">
         <f t="shared" si="9"/>
-        <v>2.9699999999999998</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>1.9432760240040001</v>
+        <v>2.4077349198269999</v>
       </c>
       <c r="B52" s="1">
-        <v>1.664073052674</v>
+        <v>0.85377486412800019</v>
       </c>
       <c r="C52" s="4">
         <f t="shared" si="4"/>
@@ -2405,35 +2405,35 @@
       </c>
       <c r="D52" s="4">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E52" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>2-2</v>
+        <v>2-1</v>
       </c>
       <c r="F52" s="3" t="str">
         <f>VLOOKUP(E52,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="H52" s="2">
         <f t="shared" si="7"/>
-        <v>1.94</v>
+        <v>2.41</v>
       </c>
       <c r="I52" s="2">
         <f t="shared" si="8"/>
-        <v>1.66</v>
+        <v>0.85</v>
       </c>
       <c r="J52" s="2">
         <f t="shared" si="9"/>
-        <v>3.5999999999999996</v>
+        <v>3.2600000000000002</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>1.236579060045</v>
+        <v>1.412790873312</v>
       </c>
       <c r="B53" s="1">
-        <v>1.0400925314579998</v>
+        <v>2.0881823538050002</v>
       </c>
       <c r="C53" s="4">
         <f t="shared" si="4"/>
@@ -2441,39 +2441,39 @@
       </c>
       <c r="D53" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E53" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F53" s="3" t="str">
         <f>VLOOKUP(E53,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="H53" s="2">
         <f t="shared" si="7"/>
-        <v>1.24</v>
+        <v>1.41</v>
       </c>
       <c r="I53" s="2">
         <f t="shared" si="8"/>
-        <v>1.04</v>
+        <v>2.09</v>
       </c>
       <c r="J53" s="2">
         <f t="shared" si="9"/>
-        <v>2.2800000000000002</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>1.7767109351900001</v>
+        <v>1.1100785431319999</v>
       </c>
       <c r="B54" s="1">
-        <v>1.4263304742780001</v>
+        <v>1.1933417017700001</v>
       </c>
       <c r="C54" s="4">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D54" s="4">
         <f t="shared" si="5"/>
@@ -2481,43 +2481,43 @@
       </c>
       <c r="E54" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F54" s="3" t="str">
         <f>VLOOKUP(E54,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="H54" s="2">
         <f t="shared" si="7"/>
-        <v>1.78</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="I54" s="2">
         <f t="shared" si="8"/>
-        <v>1.43</v>
+        <v>1.19</v>
       </c>
       <c r="J54" s="2">
         <f t="shared" si="9"/>
-        <v>3.21</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>1.9381073865420002</v>
+        <v>2.5115837750640004</v>
       </c>
       <c r="B55" s="1">
-        <v>0.38039384005599997</v>
+        <v>0.67495486646000002</v>
       </c>
       <c r="C55" s="4">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D55" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>2-0</v>
+        <v>3-1</v>
       </c>
       <c r="F55" s="3" t="str">
         <f>VLOOKUP(E55,cs_lookup!$A$2:$B$54,2,FALSE)</f>
@@ -2525,23 +2525,23 @@
       </c>
       <c r="H55" s="2">
         <f t="shared" si="7"/>
-        <v>1.94</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="I55" s="2">
         <f t="shared" si="8"/>
-        <v>0.38</v>
+        <v>0.67</v>
       </c>
       <c r="J55" s="2">
         <f t="shared" si="9"/>
-        <v>2.3199999999999998</v>
+        <v>3.1799999999999997</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>0.89864697351</v>
+        <v>1.3454913080699999</v>
       </c>
       <c r="B56" s="1">
-        <v>1.0999540588050001</v>
+        <v>0.90393094343999991</v>
       </c>
       <c r="C56" s="4">
         <f t="shared" si="4"/>
@@ -2561,23 +2561,23 @@
       </c>
       <c r="H56" s="2">
         <f t="shared" si="7"/>
+        <v>1.35</v>
+      </c>
+      <c r="I56" s="2">
+        <f t="shared" si="8"/>
         <v>0.9</v>
       </c>
-      <c r="I56" s="2">
-        <f t="shared" si="8"/>
-        <v>1.1000000000000001</v>
-      </c>
       <c r="J56" s="2">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>1.59134151605</v>
+        <v>1.8836449744320001</v>
       </c>
       <c r="B57" s="1">
-        <v>1.8803087423339997</v>
+        <v>0.57860723250000001</v>
       </c>
       <c r="C57" s="4">
         <f t="shared" si="4"/>
@@ -2585,35 +2585,35 @@
       </c>
       <c r="D57" s="4">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E57" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>2-2</v>
+        <v>2-1</v>
       </c>
       <c r="F57" s="3" t="str">
         <f>VLOOKUP(E57,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="H57" s="2">
         <f t="shared" si="7"/>
-        <v>1.59</v>
+        <v>1.88</v>
       </c>
       <c r="I57" s="2">
         <f t="shared" si="8"/>
-        <v>1.88</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="J57" s="2">
         <f t="shared" si="9"/>
-        <v>3.4699999999999998</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>1.248150425522</v>
+        <v>0.80095328198600013</v>
       </c>
       <c r="B58" s="1">
-        <v>1.5668683971159998</v>
+        <v>0.21934379615999999</v>
       </c>
       <c r="C58" s="4">
         <f t="shared" si="4"/>
@@ -2621,71 +2621,71 @@
       </c>
       <c r="D58" s="4">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E58" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-2</v>
+        <v>1-0</v>
       </c>
       <c r="F58" s="3" t="str">
         <f>VLOOKUP(E58,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H58" s="2">
         <f t="shared" si="7"/>
-        <v>1.25</v>
+        <v>0.8</v>
       </c>
       <c r="I58" s="2">
         <f t="shared" si="8"/>
-        <v>1.57</v>
+        <v>0.22</v>
       </c>
       <c r="J58" s="2">
         <f t="shared" si="9"/>
-        <v>2.8200000000000003</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>0.94655286869000022</v>
+        <v>2.2466374330400001</v>
       </c>
       <c r="B59" s="1">
-        <v>0.37605285937900007</v>
+        <v>1.6500044220000001</v>
       </c>
       <c r="C59" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D59" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E59" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-0</v>
+        <v>2-2</v>
       </c>
       <c r="F59" s="3" t="str">
         <f>VLOOKUP(E59,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="H59" s="2">
         <f t="shared" si="7"/>
-        <v>0.95</v>
+        <v>2.25</v>
       </c>
       <c r="I59" s="2">
         <f t="shared" si="8"/>
-        <v>0.38</v>
+        <v>1.65</v>
       </c>
       <c r="J59" s="2">
         <f t="shared" si="9"/>
-        <v>1.33</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>0.624002989896</v>
+        <v>0.94655286869000022</v>
       </c>
       <c r="B60" s="1">
-        <v>0.18799309757999999</v>
+        <v>0.84610226754800011</v>
       </c>
       <c r="C60" s="4">
         <f t="shared" si="4"/>
@@ -2693,39 +2693,39 @@
       </c>
       <c r="D60" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-0</v>
+        <v>1-1</v>
       </c>
       <c r="F60" s="3" t="str">
         <f>VLOOKUP(E60,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="H60" s="2">
         <f t="shared" si="7"/>
-        <v>0.62</v>
+        <v>0.95</v>
       </c>
       <c r="I60" s="2">
         <f t="shared" si="8"/>
-        <v>0.19</v>
+        <v>0.85</v>
       </c>
       <c r="J60" s="2">
         <f t="shared" si="9"/>
-        <v>0.81</v>
+        <v>1.7999999999999998</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>1.6641413094020001</v>
+        <v>0.87375307533800006</v>
       </c>
       <c r="B61" s="1">
-        <v>0.75215016419699998</v>
+        <v>1.1281585781369998</v>
       </c>
       <c r="C61" s="4">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" s="4">
         <f t="shared" si="5"/>
@@ -2733,43 +2733,43 @@
       </c>
       <c r="E61" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>2-1</v>
+        <v>1-1</v>
       </c>
       <c r="F61" s="3" t="str">
         <f>VLOOKUP(E61,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="H61" s="2">
         <f t="shared" si="7"/>
-        <v>1.66</v>
+        <v>0.87</v>
       </c>
       <c r="I61" s="2">
         <f t="shared" si="8"/>
-        <v>0.75</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J61" s="2">
         <f t="shared" si="9"/>
-        <v>2.41</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>0.35101209686399998</v>
+        <v>0.68654884555399998</v>
       </c>
       <c r="B62" s="1">
-        <v>0.37016210139200001</v>
+        <v>0.65810916996799995</v>
       </c>
       <c r="C62" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D62" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>0-0</v>
+        <v>1-1</v>
       </c>
       <c r="F62" s="3" t="str">
         <f>VLOOKUP(E62,cs_lookup!$A$2:$B$54,2,FALSE)</f>
@@ -2777,27 +2777,27 @@
       </c>
       <c r="H62" s="2">
         <f t="shared" si="7"/>
-        <v>0.35</v>
+        <v>0.69</v>
       </c>
       <c r="I62" s="2">
         <f t="shared" si="8"/>
-        <v>0.37</v>
+        <v>0.66</v>
       </c>
       <c r="J62" s="2">
         <f t="shared" si="9"/>
-        <v>0.72</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>1.0909898755199998</v>
+        <v>1.5730055670800003</v>
       </c>
       <c r="B63" s="1">
-        <v>1.0137902675199999</v>
+        <v>0.90494999279999999</v>
       </c>
       <c r="C63" s="4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D63" s="4">
         <f t="shared" si="5"/>
@@ -2805,31 +2805,31 @@
       </c>
       <c r="E63" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>2-1</v>
       </c>
       <c r="F63" s="3" t="str">
         <f>VLOOKUP(E63,cs_lookup!$A$2:$B$54,2,FALSE)</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="H63" s="2">
         <f t="shared" si="7"/>
-        <v>1.0900000000000001</v>
+        <v>1.57</v>
       </c>
       <c r="I63" s="2">
         <f t="shared" si="8"/>
-        <v>1.01</v>
+        <v>0.9</v>
       </c>
       <c r="J63" s="2">
         <f t="shared" si="9"/>
-        <v>2.1</v>
+        <v>2.4700000000000002</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>0.94213761693800002</v>
+        <v>1.076728705072</v>
       </c>
       <c r="B64" s="1">
-        <v>0.66566421862499991</v>
+        <v>1.0142454813749999</v>
       </c>
       <c r="C64" s="4">
         <f t="shared" si="4"/>
@@ -2849,23 +2849,23 @@
       </c>
       <c r="H64" s="2">
         <f t="shared" si="7"/>
-        <v>0.94</v>
+        <v>1.08</v>
       </c>
       <c r="I64" s="2">
         <f t="shared" si="8"/>
-        <v>0.67</v>
+        <v>1.01</v>
       </c>
       <c r="J64" s="2">
         <f t="shared" si="9"/>
-        <v>1.6099999999999999</v>
+        <v>2.09</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>0.99855589519400001</v>
+        <v>1.076728705072</v>
       </c>
       <c r="B65" s="1">
-        <v>0.56410151178800017</v>
+        <v>1.7931342279390001</v>
       </c>
       <c r="C65" s="4">
         <f t="shared" si="4"/>
@@ -2873,143 +2873,462 @@
       </c>
       <c r="D65" s="4">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E65" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
       <c r="F65" s="3" t="str">
         <f>VLOOKUP(E65,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H65" s="2">
+        <f t="shared" si="7"/>
+        <v>1.08</v>
+      </c>
+      <c r="I65" s="2">
+        <f t="shared" si="8"/>
+        <v>1.79</v>
+      </c>
+      <c r="J65" s="2">
+        <f t="shared" si="9"/>
+        <v>2.87</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>1.2920144500590001</v>
+      </c>
+      <c r="B66" s="1">
+        <v>1.304062556391</v>
+      </c>
+      <c r="C66" s="4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D66" s="4">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E66" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1-1</v>
+      </c>
+      <c r="F66" s="3" t="str">
+        <f>VLOOKUP(E66,cs_lookup!$A$2:$B$54,2,FALSE)</f>
         <v>X</v>
       </c>
-      <c r="H65" s="2">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="I65" s="2">
-        <f t="shared" si="8"/>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="J65" s="2">
-        <f t="shared" si="9"/>
-        <v>1.56</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="3"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
+      <c r="H66" s="2">
+        <f t="shared" si="7"/>
+        <v>1.29</v>
+      </c>
+      <c r="I66" s="2">
+        <f t="shared" si="8"/>
+        <v>1.3</v>
+      </c>
+      <c r="J66" s="2">
+        <f t="shared" si="9"/>
+        <v>2.59</v>
+      </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="3"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
+      <c r="A67" s="1">
+        <v>1.8844538076959998</v>
+      </c>
+      <c r="B67" s="1">
+        <v>0.85590756996000006</v>
+      </c>
+      <c r="C67" s="4">
+        <f t="shared" ref="C67:C77" si="10">ROUND(A67,0)</f>
+        <v>2</v>
+      </c>
+      <c r="D67" s="4">
+        <f t="shared" ref="D67:D77" si="11">ROUND(B67,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E67" s="5" t="str">
+        <f t="shared" ref="E67:E77" si="12">CONCATENATE(C67,"-",D67)</f>
+        <v>2-1</v>
+      </c>
+      <c r="F67" s="3" t="str">
+        <f>VLOOKUP(E67,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H67" s="2">
+        <f t="shared" ref="H67:H77" si="13">ROUND(A67,2)</f>
+        <v>1.88</v>
+      </c>
+      <c r="I67" s="2">
+        <f t="shared" ref="I67:I77" si="14">ROUND(B67,2)</f>
+        <v>0.86</v>
+      </c>
+      <c r="J67" s="2">
+        <f t="shared" ref="J67:J77" si="15">SUM(H67:I67)</f>
+        <v>2.7399999999999998</v>
+      </c>
     </row>
     <row r="68" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="5"/>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
+      <c r="A68" s="2">
+        <v>1.8303788025950001</v>
+      </c>
+      <c r="B68" s="2">
+        <v>0.43472561252399999</v>
+      </c>
+      <c r="C68" s="4">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="D68" s="4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E68" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>2-0</v>
+      </c>
+      <c r="F68" s="3" t="str">
+        <f>VLOOKUP(E68,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="G68"/>
+      <c r="H68" s="2">
+        <f t="shared" si="13"/>
+        <v>1.83</v>
+      </c>
+      <c r="I68" s="2">
+        <f t="shared" si="14"/>
+        <v>0.43</v>
+      </c>
+      <c r="J68" s="2">
+        <f t="shared" si="15"/>
+        <v>2.2600000000000002</v>
+      </c>
     </row>
     <row r="69" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
-      <c r="E69" s="5"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
-      <c r="J69" s="2"/>
+      <c r="A69" s="2">
+        <v>0.96911083424</v>
+      </c>
+      <c r="B69" s="2">
+        <v>1.0142454813749999</v>
+      </c>
+      <c r="C69" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="D69" s="4">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E69" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>1-1</v>
+      </c>
+      <c r="F69" s="3" t="str">
+        <f>VLOOKUP(E69,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="G69"/>
+      <c r="H69" s="2">
+        <f t="shared" si="13"/>
+        <v>0.97</v>
+      </c>
+      <c r="I69" s="2">
+        <f t="shared" si="14"/>
+        <v>1.01</v>
+      </c>
+      <c r="J69" s="2">
+        <f t="shared" si="15"/>
+        <v>1.98</v>
+      </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="3"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
+      <c r="A70" s="1">
+        <v>0.64605722171900004</v>
+      </c>
+      <c r="B70" s="1">
+        <v>0.95097031358400008</v>
+      </c>
+      <c r="C70" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="D70" s="4">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E70" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>1-1</v>
+      </c>
+      <c r="F70" s="3" t="str">
+        <f>VLOOKUP(E70,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H70" s="2">
+        <f t="shared" si="13"/>
+        <v>0.65</v>
+      </c>
+      <c r="I70" s="2">
+        <f t="shared" si="14"/>
+        <v>0.95</v>
+      </c>
+      <c r="J70" s="2">
+        <f t="shared" si="15"/>
+        <v>1.6</v>
+      </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="3"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
-      <c r="J71" s="2"/>
+      <c r="A71" s="1">
+        <v>1.3105518354500001</v>
+      </c>
+      <c r="B71" s="1">
+        <v>0.50143344279800017</v>
+      </c>
+      <c r="C71" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="D71" s="4">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E71" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>1-1</v>
+      </c>
+      <c r="F71" s="3" t="str">
+        <f>VLOOKUP(E71,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H71" s="2">
+        <f t="shared" si="13"/>
+        <v>1.31</v>
+      </c>
+      <c r="I71" s="2">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="J71" s="2">
+        <f t="shared" si="15"/>
+        <v>1.81</v>
+      </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="3"/>
-      <c r="H72" s="2"/>
-      <c r="I72" s="2"/>
-      <c r="J72" s="2"/>
+      <c r="A72" s="1">
+        <v>1.144166591282</v>
+      </c>
+      <c r="B72" s="1">
+        <v>0.31338479038899997</v>
+      </c>
+      <c r="C72" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="D72" s="4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E72" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>1-0</v>
+      </c>
+      <c r="F72" s="3" t="str">
+        <f>VLOOKUP(E72,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H72" s="2">
+        <f t="shared" si="13"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="I72" s="2">
+        <f t="shared" si="14"/>
+        <v>0.31</v>
+      </c>
+      <c r="J72" s="2">
+        <f t="shared" si="15"/>
+        <v>1.45</v>
+      </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="3"/>
+      <c r="A73" s="1">
+        <v>1.373097691108</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0.62676958077800005</v>
+      </c>
+      <c r="C73" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="D73" s="4">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E73" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>1-1</v>
+      </c>
+      <c r="F73" s="3" t="str">
+        <f>VLOOKUP(E73,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H73" s="2">
+        <f t="shared" si="13"/>
+        <v>1.37</v>
+      </c>
+      <c r="I73" s="2">
+        <f t="shared" si="14"/>
+        <v>0.63</v>
+      </c>
+      <c r="J73" s="2">
+        <f t="shared" si="15"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="3"/>
+      <c r="A74" s="1">
+        <v>0.90105716386400003</v>
+      </c>
+      <c r="B74" s="1">
+        <v>1.7451046768680003</v>
+      </c>
+      <c r="C74" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="D74" s="4">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="E74" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>1-2</v>
+      </c>
+      <c r="F74" s="3" t="str">
+        <f>VLOOKUP(E74,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H74" s="2">
+        <f t="shared" si="13"/>
+        <v>0.9</v>
+      </c>
+      <c r="I74" s="2">
+        <f t="shared" si="14"/>
+        <v>1.75</v>
+      </c>
+      <c r="J74" s="2">
+        <f t="shared" si="15"/>
+        <v>2.65</v>
+      </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="3"/>
+      <c r="A75" s="1">
+        <v>0.39949116876000007</v>
+      </c>
+      <c r="B75" s="1">
+        <v>1.7644524824000005</v>
+      </c>
+      <c r="C75" s="4">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D75" s="4">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="E75" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>0-2</v>
+      </c>
+      <c r="F75" s="3" t="str">
+        <f>VLOOKUP(E75,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H75" s="2">
+        <f t="shared" si="13"/>
+        <v>0.4</v>
+      </c>
+      <c r="I75" s="2">
+        <f t="shared" si="14"/>
+        <v>1.76</v>
+      </c>
+      <c r="J75" s="2">
+        <f t="shared" si="15"/>
+        <v>2.16</v>
+      </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="3"/>
+      <c r="A76" s="1">
+        <v>0.53836435253600001</v>
+      </c>
+      <c r="B76" s="1">
+        <v>1.6301103374230002</v>
+      </c>
+      <c r="C76" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="D76" s="4">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="E76" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>1-2</v>
+      </c>
+      <c r="F76" s="3" t="str">
+        <f>VLOOKUP(E76,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H76" s="2">
+        <f t="shared" si="13"/>
+        <v>0.54</v>
+      </c>
+      <c r="I76" s="2">
+        <f t="shared" si="14"/>
+        <v>1.63</v>
+      </c>
+      <c r="J76" s="2">
+        <f t="shared" si="15"/>
+        <v>2.17</v>
+      </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="3"/>
+      <c r="A77" s="1">
+        <v>0.93606559832500014</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0.65810916996799995</v>
+      </c>
+      <c r="C77" s="4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="D77" s="4">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="E77" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v>1-1</v>
+      </c>
+      <c r="F77" s="3" t="str">
+        <f>VLOOKUP(E77,cs_lookup!$A$2:$B$54,2,FALSE)</f>
+        <v>X</v>
+      </c>
+      <c r="H77" s="2">
+        <f t="shared" si="13"/>
+        <v>0.94</v>
+      </c>
+      <c r="I77" s="2">
+        <f t="shared" si="14"/>
+        <v>0.66</v>
+      </c>
+      <c r="J77" s="2">
+        <f t="shared" si="15"/>
+        <v>1.6</v>
+      </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>

</xml_diff>